<commit_message>
Add new data holy persons. Edit holy person page.
</commit_message>
<xml_diff>
--- a/public/data/holy_persons.xlsx
+++ b/public/data/holy_persons.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Лист1" sheetId="6" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Святые!$A$1:$V$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Святые!$A$1:$V$97</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1458" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1684" uniqueCount="1216">
   <si>
     <t>Отчество</t>
   </si>
@@ -5002,6 +5002,697 @@
   </si>
   <si>
     <t>:vEparchy ,</t>
+  </si>
+  <si>
+    <t>Климент I, Римский</t>
+  </si>
+  <si>
+    <t>I век</t>
+  </si>
+  <si>
+    <t>Рим</t>
+  </si>
+  <si>
+    <t>середина I века</t>
+  </si>
+  <si>
+    <t>Херсонес</t>
+  </si>
+  <si>
+    <t>конец I века</t>
+  </si>
+  <si>
+    <t>Апостол от 70</t>
+  </si>
+  <si>
+    <t>08. 12.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Согласно православному житию святого Климента, он происходил из знатной римской семьи. Вскоре после рождения Климента (30-е годы), его мать, Матфидия, и два брата отправились по морю из Рима в Афины. Их корабль потерпел крушение, но они выжили, хотя потеряли друг друга. Мать Климента, оплакивая потерю детей, осталась на одном из островов Восточного Средиземноморья; малолетние же братья оказались в Иудее и были там усыновлены. Климент же взрослел в Риме, изучая науки и скорбя о пропавших родичах. Ни языческая религия, ни философия не могли дать ему удовлетворительного ответа на вопрос, что происходит с людьми после смерти. Когда Клименту исполнилось 24 года, он услышал о пришествии Христа в мир и решил узнать подробнее о его учении, для чего отправился на восток. В Александрии он слушал проповеди апостола Варнавы, а в Иудее нашёл святого апостола Петра, принял от него крещение и присоединился к его. Климент стал одним из ближайших сподвижников Петра и был рукоположён им во епископы, а около 91 года, после смерти епископа Анаклета, возглавил Римскую церковь. В период очередной волны гонений на христианство Климент был поставлен перед выбором: принести жертву языческим богам или быть отправленным в изгнание на каторжные работы. В каменоломнях возле крупного античного города Херсонеса Таврического (нынешний Севастополь), отождествляемых обычно с Инкерманскими каменоломнями. Климент всякий день крестил до 500 язычников, и число христиан так увеличилось, что для них потребовалось устроить до 75 новых церквей; языческие идолы были разбиты, а капища — разрушены. В Херсонес для наведения порядка император Траян направил специального посланника, который приказал привязать Климента к якорю и утопить в море, дабы последователи не нашли его тела. Однако по молитвам учеников Климента и остального народа море отступило от берега на три стадия (около 500 м), и люди нашли тело мученика.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Климент_I#Житие_Святого_Климента</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Климент_I#/media/Файл:Pope_Clement_I.jpg</t>
+  </si>
+  <si>
+    <t>97-101 гг.</t>
+  </si>
+  <si>
+    <t>Иусти́н Филосо́ф</t>
+  </si>
+  <si>
+    <t>около 100 г.</t>
+  </si>
+  <si>
+    <t>Сирия Паленстинская</t>
+  </si>
+  <si>
+    <t>II век</t>
+  </si>
+  <si>
+    <t>Эфес</t>
+  </si>
+  <si>
+    <t>Ii век</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14. 06. </t>
+  </si>
+  <si>
+    <t>Апологет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родился около 100 года в городе Флавия Неаполис в римской провинции Сирии Палестинской. Иустин в книге «Диалог с Трифоном иудеем» подробно описывает своё обучение. Сначала он занимался философией у стоического философа, но вскоре разочаровался в стоической школе ввиду того, что она, по мнению Иустина, не считала познания о Боге необходимыми. Тем не менее, уже став христианином, Иустин считал Сократа и стоиков до Рождества Христова христианами до Христа. Затем Иустин познакомился с перипатетиком, но ушел от него после того, как тот потребовал плату за обучение. Иустин беседовал с неким знаменитым пифагорейцем, но не был допущен к обучению в этой школе ввиду отсутствия у Иустина познаний в области музыки, астрономии и геометрии. После этого он познакомился с платоником, с которым занимался философией долгое время. Таким образом, на Иустина оказал значительное влияние платонизм промежуточного периода (Средний платонизм) Но наиболее важной в жизни Иустина оказалась встреча с пожилым человеком, вероятно, палестинским или сирийским христианином. Иустин принимает крещение, вероятно, в промежуток между 132 и 137 г. и занимается активной миссионерской деятельностью. Иустин много путешествует, в частности, он посещает Александрию и Эфес. В правление Антонина Пия прибывает в Рим, где основывает собственную официально — философскую школу, но фактически — катехизическую школу, среди учеников которой был Татиан. Согласно «Мученическим актам», сохранившимся в сборнике Симеона Метафраста, римский префект Рустик расспрашивал Иустина о его вере и христианском образе жизни, а также убеждал вернуться к почитанию эллинских богов, на что получил отказ. Иустин вместе с шестью своими учениками подверглись бичеванию, а затем были обезглавлены. Таким образом, Иустин был казнён около 165 г.[21]
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иустин_Философ</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иустин_Философ#/media/Файл:Justin_filozof.jpg</t>
+  </si>
+  <si>
+    <t>165 г.</t>
+  </si>
+  <si>
+    <t>Киприа́н Карфаге́нский</t>
+  </si>
+  <si>
+    <t>около 200 г.</t>
+  </si>
+  <si>
+    <t>Карфаген</t>
+  </si>
+  <si>
+    <t>Кафраген</t>
+  </si>
+  <si>
+    <t>Святой</t>
+  </si>
+  <si>
+    <t>13.09.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Вырос в языческом окружении, до 246 г. был известен как преуспевающий юрист. Через два года после крещения по требованию паствы был избран в епископы (что нарушало принятые тогда нормы). Через пару месяцев началось жестокое гонение императора Деция на христиан, многие из которых отступили от веры, если не на деле, то на словах. По поводу условий их приёма обратно в лоно Церкви развернулись большие споры. Киприан, который последовательно отстаивал необходимость соборов как высшей инстанции для разрешения церковных дел, на соборе в Карфагене сумел провести точку зрения о том, что полномочия церкви включают в себя и отпущение смертных грехов (даже таких, как отступничество). Впоследствии взгляды Киприана по этому вопросу стали общепринятыми.В 254 г. Киприан, который до этого подчёркивал верховенство римского епископа среди прочих, столкнулся с папой Стефаном по вопросу о допустимости возвращения на свои посты испанских епископов, которые во время гонений приносили жертвы языческим божествам. За несколько месяцев спор принял более серьёзный оборот и стал грозить церкви расколом. Дело неминуемо шло к разрыву между Карфагеном и Римом, когда папа Стефан был казнён. Во время гонения императора Валериан I Киприан был вызван к проконсулу Аспазию Патерну, допрошен и отправлен в ссылку (30 августа 257 г.). На следующий год гонения усилились, Киприан вновь предстал перед судом и был казнён. Был причтён к числу отцов Единой Церкви.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Киприан_Карфагенский</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Киприан_Карфагенский#/media/Файл:Heiliger_Cyprianus.jpg</t>
+  </si>
+  <si>
+    <t>14. 09. 258</t>
+  </si>
+  <si>
+    <t>Василий Великий</t>
+  </si>
+  <si>
+    <t>около 330 г.</t>
+  </si>
+  <si>
+    <t>Кесарии Каппадокийской</t>
+  </si>
+  <si>
+    <t>Афины</t>
+  </si>
+  <si>
+    <t>350-355 гг.</t>
+  </si>
+  <si>
+    <t>14.01./ 12. 02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родился святой Василий около 330 года в Кесарии, административном центре Каппадокии, и происходил из известного рода, славившегося как знатностью и богатством, так и дарованиями и ревностью христианской веры. Василий получил прекрасное образование в Кесарии и Константинополе, а закончил его в Афинах, где пять лет (350—355) обучался в школе риторов Проэресия. По возвращении в Кесарию Василий было посвятил себя светским делам. Вместе со своим другом Григорием Богословом поселился на семейных землях в Понте, где они изучали труды Оригена. В 356 или 357 году Василий пустился в продолжительное путешествие в Сирию и Египет (Фиваида), после чего возобновил аскетическую практику. В 357 году был рукоположен в священники, после чего оставаясь в Понте, начал активно участвовать в жизни церкви. В 360 году в качестве чтеца сопровождал каппадокийских епископов на Собор в Константинополь. В 364 году Василий был рукоположён во пресвитеры и сделался советником Евсевия, сменившего Диания в качестве епископа.В 365 году Василий вернулся в Кесарию и взял управление епархией в свои руки.. Несмотря на противодействие ряда епископов, по смерти Евсевия в 370 году Василий заступил на место митрополита Каппадокийского и ревностно принялся за искоренение арианства в Малой Азии. Антиарианская деятельность Василия привела его к столкновению с Валентом. Во время путешествия императора по Каппадокии епископ наотрез отказался признать правоту арианского учения. В ответ Валент разделил Каппадокию на две провинции, что привело к сокращению канонической территории Василия и подорвало его позиции в церкви. Тем не менее Василию удалось продвинуть на место епископов ключевых городов своих соратников Григория Нисского и Григория Богослова. Гибель Валента в битве при Адрианополе изменила баланс сил в государстве и церкви, но Василий воспользоваться этим не успел. Он умер в первый день нового 379 года и в скором времени был причислен к лику святых.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Василий_Великий</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Василий_Великий#/media/Файл:Basil_of_Caesarea_icon.jpg</t>
+  </si>
+  <si>
+    <t>379 г.</t>
+  </si>
+  <si>
+    <t>Иоа́нн Златоу́ст</t>
+  </si>
+  <si>
+    <t>около 347 г.</t>
+  </si>
+  <si>
+    <t>Антиохия</t>
+  </si>
+  <si>
+    <t>конец IV века</t>
+  </si>
+  <si>
+    <t>27.09./ 26. 11./ 09.02./ 12.02.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родился в Антиохии около 347 года, в семье чиновника. Его отец. Святитель Мелетий Антиохийский в 367 году крестил его. Через три года Иоанн был сделан чтецом. После того, как Мелетий был отправлен в ссылку императором Валентом в 372 году, Иоанн совместно с Феодором Мопсуестийским учился в местной богословской школе у пресвитеров Флавиана и Диодора Тарсийского. В 381 году епископ Мелетий Антиохийский рукоположил Иоанна в сан диакона. В 386 году Иоанн был рукоположён в пресвитеры. В 397 году, после кончины константинопольского архиепископа Нектария (управлял Константинопольской церковью с 381 по 397 г., был преемником Григория Назианзина), Иоанн был вызван из Антиохии для поставления на константинопольскую кафедру в качестве архиепископа. Иоанн оказался втянутым в конфликт с императорским двором, когда укрыл в церкви свергнутого за корыстолюбие и несправедливые поступки консула Евтропия. И, в частности, с женой императора: когда императрица Евдоксия, жена императора Аркадия (395—408), распорядилась о конфискации собственности у вдовы и детей опального вельможи, Иоанн стал на их защиту. Императрица не уступила и затаила гнев на архипастыря. Иоанн был обвинён в оригенизме Александрийским архиепископством в глазах императора. Император по недальновидным и своекорыстным соображениям встал на сторону Александрийского архиепископства.  В марте 404 года состоялся собор, постановивший изгнать Иоанна. Столкнувшись с перспективой изгнания, Иоанн обратился за помощью к Римскому Папе Иннокентию I, а также к архиепископу Медиолана св. Венерию и епископу Аквилеи св. Хромацию. Иннокентий I отправил в Константинополь делегацию под руководством св. Гауденция Брешийского, который ранее в Антиохии встречался с Иоанном и был с ним дружен. Однако в Греции папских посланцев сперва арестовали, затем хотели подкупить и в конце концов депортировали. Несмотря на их неудачу, Иоанн написал Гауденцию благодарственное письмо. Император Флавий Аркадий назначил город Кукус (лат. Cucusus, ныне — Гёксун в Турции) в провинции Армения Вторая местом ссылки Иоанна Златоуста. Находясь в Армении, Иоанн старался укрепить  своих  последователей.  В  своих письмах (их сохранилось 245) епископам Азии, Африки, Европы и своим друзьям в Константинополе, он утешал страдающих, наставлял и поддерживал своих приверженцев. Зимой 406 года Иоанн был болезнью прикован к постели. Но враги его не унимались. Из столицы пришёл приказ перевести его в глухой Пифиунт (Пицунду, ныне в Абхазии). Истощённый болезнями Златоуст, в сопровождении конвоя, три месяца в дождь и зной совершал свой последний переход, подвергаясь издевательствам и жестокому обращению стражей. В Команах силы оставили его. Причастившись Святых Таин, он, со словами «Слава Богу за всё!» скончался 14 сентября 407 года. Иоанн был погребён в Команах Понтийских, в мартирии мученика Василиска, рядом с могилой мученика Василиска, на территории современной Турции. 
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Златоуст</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Златоуст#/media/Файл:Johnchrysostom.jpg</t>
+  </si>
+  <si>
+    <t>14. 09. 407 г.</t>
+  </si>
+  <si>
+    <t>погребён в Команах Понтийских</t>
+  </si>
+  <si>
+    <t>Варсоно́фий Вели́кий</t>
+  </si>
+  <si>
+    <t>вторая половина V  века</t>
+  </si>
+  <si>
+    <t>Египет</t>
+  </si>
+  <si>
+    <t>Газа Палестинская</t>
+  </si>
+  <si>
+    <t>конец V - начало VI вв.</t>
+  </si>
+  <si>
+    <t>19. 02.</t>
+  </si>
+  <si>
+    <t>Монах</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Варсонофий родился в Египте. По некоторым данным, детство и юность провёл в крупном городе, был хорошо образован, знал несколько языков. Впоследствии удалился в монастырь Аввы Серида в окрестностях Газы Палестинской, где жил в маленькой келлии в пещере вблизи монастыря. Более 50 лет святой жил уединённо в полном безмолвии, питаясь только хлебом и водой, в стенах монастыря и в пустыне. Варсонофий обладал даром чудотворения, в том числе воскрешения умерших. В затворе преподобный Варсонофий предался молитве и достиг высокой степени духовного совершенства. О жизни, подвигах и благодатных дарованиях Варсонофия сохранились свидетельства в рукописях. В славянских списках XV—XVII веков есть наставления в форме ответов на вопросы, которые ему задавали ученики и мирские люди. В XVIII веке стараниями молдавского старца схиархимандрита Паисия Величковского были найдены на Афоне наиболее полные две древнейшие пергаменные греческие рукописи «Ответов» Варсонофия. Они были при жизни старца Паисия переведены на молдавский и славянский языки. Издание этих рукописей, так же как и перевод на русский язык, было осуществлено в XIX веке старцами Введенской Оптиной пустыни. Наставления Варсонофия показывают степень его нравственного совершенства, любви к людям, содержат скупые факты жизни. Неизвестно точное время кончины преподобного Варсонофия: одни называют годом его смерти 563, другие говорят более осторожно — до 600 года. Его мощи в 850 году были привезены в Италию, где и хранятся в городе Ория, покровителем которого он считается в Католической церкви.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Варсонофий_Великий</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Варсонофий_Великий#/media/Файл:Statua_S_Barsanofio_Oria.jpg</t>
+  </si>
+  <si>
+    <t>около 563 г.</t>
+  </si>
+  <si>
+    <t>Иоа́нн Ле́ствичник</t>
+  </si>
+  <si>
+    <t>579 г.</t>
+  </si>
+  <si>
+    <t>595 г.</t>
+  </si>
+  <si>
+    <t>4-е воскресение Великого поста</t>
+  </si>
+  <si>
+    <t>Отшельник</t>
+  </si>
+  <si>
+    <t>Родился в Константинополе и получил хорошее образование в юности. В 16 лет переехал в Египет на Синайскую гору и предал себя в повиновение старцу Мартирию. Через четыре года послушания принял монашеский постриг. После смерти старца Мартирия, в послушании у которого Иоанн прожил около 19 лет, святой избрал отшельническую жизнь и провёл ещё 40 лет в пустыне Фола. Впоследствии в возрасте 65 лет Иоанн Лествичник был избран братией игуменом Синайской обители и управлял монастырём четыре года. Святой умер, по данным из некоторых источников, в 649 году в возрасте 70 лет. Местонахождение мощей Иоанна неизвестно.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Лествичник#Иконография</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Лествичник#/media/Файл:John_Climacus.jpg</t>
+  </si>
+  <si>
+    <t>649 г.</t>
+  </si>
+  <si>
+    <t>Иоа́нн Дамаски́н</t>
+  </si>
+  <si>
+    <t>около 675 г.</t>
+  </si>
+  <si>
+    <t>Дамаск</t>
+  </si>
+  <si>
+    <t>Обитель Саввы Освященного</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17. 12. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Его тёзка-дед и его отец Серджун ибн Мансур служили в Дамаске в звании «великого логофета», то есть откупщика, и при ромейском (византийском) владычестве, и при персидской оккупации, дед участвовал в передаче власти арабам, а отец служил при дворе халифа Абд ал-Малика ибн Марвана. Впоследствии его сменил сам Иоанн. По преданию, Иоанн учился точным наукам и музыке вместе с братом Косьмой (впоследствии — епископ Маюмский) у некоего пленного инока из Калабрии (тоже по имени Косьма). После введения арабского языка (вместо греческого) как единственного государственного, в том числе, налоговой администрации, около 706 года или в 710-х годах принял пострижение в монастыре святого Саввы близ Иерусалима и, вероятно, был рукоположён во священника. В период иконоборчества выступал в защиту почитания икон, автор «Трёх защитительных слов в поддержку иконопочитания», в которых иконоборчество понимается как христологическая ересь, а также впервые различается «поклонение», подобающее только Богу, и «почитание», оказываемое тварным вещам, в том числе и иконам. Иконоборческий собор 754 года четырежды подверг Иоанна анафеме, но VII Вселенский собор подтвердил верность его учения. Скончался около 753 года (по другим данным, около 780 года) и был погребён в лавре Саввы Освященного возле раки с мощами преподобного Саввы.
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Дамаскин</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Иоанн_Дамаскин#/media/Файл:Ioann_Damaskin_ikona.jpg</t>
+  </si>
+  <si>
+    <t>753-780 гг.</t>
+  </si>
+  <si>
+    <t>Фео́дор Студи́т</t>
+  </si>
+  <si>
+    <t>759 г.</t>
+  </si>
+  <si>
+    <t>монастыря Саккудион</t>
+  </si>
+  <si>
+    <t>781 г.</t>
+  </si>
+  <si>
+    <t>Студийский монастырь</t>
+  </si>
+  <si>
+    <t>798 г.</t>
+  </si>
+  <si>
+    <t>828 г.</t>
+  </si>
+  <si>
+    <t>08. 02 / 24. 11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сын чиновника, Феодор получил хорошее образование под руководством матери; под влиянием дяди Платона, игумена монастыря Саккудион, 22 лет от роду постригся в этом монастыре; молодая жена его Анна также приняла монашество. Ещё при жизни Платона Феодор стал игуменом и стал известен как аскет и проповедник. В 798 году он переселился со своими учениками в Студийский монастырь. Феодор отзывался на все главные вопросы текущей политической и общественной жизни. Считая долгом пастыря и монаха идти против всякого беззакония в церковных делах, он выступил против незаконного с канонической точки зрения развода и нового брака императора Константина VI. Он был подвергнут истязаниям и изгнан, но скоро по смерти Константина вернулся в свою обитель (797). Когда возник вопрос о прощении отрешённого от сана священника, повенчавшего Константина, Феодор восстал против этого и был изгнан на один из Принцевых островов, где пробыл два года (809—811). За устроенный им крестный ход с иконами Феодор был заключён и сослан; биография, составленная двумя поколениями позже, много говорит о его мучениях и скитаниях. В темнице Феодор продолжал борьбу, апеллируя к патриархам, прежде всего к папе, которому «Христос вручил ключи веры». Новый император прекратил преследования. Феодор встречен был народом как мученик и чудотворец; но монастыря ему император не вернул. В скитаниях он скончался в 826 году, окружённый учениками. 
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Феодор_Студит</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Феодор_Студит#/media/Файл:Studite.jpg</t>
+  </si>
+  <si>
+    <t>826 г.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Людми́ла, княгиня Чешская</t>
+  </si>
+  <si>
+    <t>около 860г.</t>
+  </si>
+  <si>
+    <t>Мельник</t>
+  </si>
+  <si>
+    <t>Тетин</t>
+  </si>
+  <si>
+    <t>1143-1144</t>
+  </si>
+  <si>
+    <t>29. 09.</t>
+  </si>
+  <si>
+    <t>Княгиня</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Людмила, согласно христианской легенде — дочь князя пшован Славибора. Жена Борживоя I, первого христианского князя Чехии. Людмила и Борживой были крещены около 871 года епископом Мефодием в Велеграде, при дворе князя Святополка (874—885). После возвращения совместно правили более семи лет. Так как многие чехи были недовольны политикой христианизации, проводимой Борживоем I, в 883 или в 884 году против князя поднялось восстание. Борживой бежал к князю Святополку I Моравскому и вскоре с его помощью подавил восстание. В честь победы он построил в своей столице церковь Св. Девы Марии. Когда через несколько лет Борживой умер, его земли перешли под непосредственную власть князя Святополка I , однако, после его смерти в 894 году, князем чехов стал старший сын Борживоя, Спытигнев I, который скончался в 915 году. Правление принял следующий сын, Вратислав, женатый на Драгомире, номинальной христианке, поддерживающей языческие традиции. Вратислав скончался, оставив наследником восьмилетнего сына Вацлава (Венцеслава, Вячеслава). Вацлав был воспитан святой Людмилой в духе христианства, тогда как его брат Болеслав, воспитанный матерью, — в традициях язычества. После смерти Вратислава Людмила продолжала оказывать влияние на внука. Она действовала как регент, поддерживая Вацлава. По наущению невестки Драгомиры двое убийц в ночь с 15 на 16 сентября 921 года ворвались в покои Людмилы, и в возрасте около 60 лет она была задушена языческой знатью. Предположительно, в качестве орудия убийства была использована вуаль княгини, которая впоследствии стала её символом. Людмила стала мученицей и была причислена к лику святых в 1143—1144 годах
+</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Людмила_Чешская</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Людмила_Чешская#/media/Файл:Votivni_obraz_Ocko_-_Ludmila.jpg</t>
+  </si>
+  <si>
+    <t>15. 09. 921 г.</t>
+  </si>
+  <si>
+    <t>Симеон Новый Богослов</t>
+  </si>
+  <si>
+    <t>949 г.</t>
+  </si>
+  <si>
+    <t>Галатия</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Студийский монастырь</t>
+  </si>
+  <si>
+    <t>973 г.</t>
+  </si>
+  <si>
+    <t>25. 03.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Родился в 949 году в Малой Азии в городе Хрисополис (в настоящее время район Стамбула) в богатой и знатной семье, получил хорошее образование, но с ранних лет был склонен к уединённой монашеской жизни. В 973 году поступил в Студийский монастырь, где подвизался под руководством старца Симеона Благоговейного. </t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Симеон_Новый_Богослов</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Симеон_Новый_Богослов#/media/Файл:Simeon_novyj.jpg</t>
+  </si>
+  <si>
+    <t>1022 г.</t>
+  </si>
+  <si>
+    <t>Дионисий Ареопагит</t>
+  </si>
+  <si>
+    <t>I в.</t>
+  </si>
+  <si>
+    <t>г. Афины, Греция</t>
+  </si>
+  <si>
+    <t>57-67 гг.</t>
+  </si>
+  <si>
+    <t>Германия</t>
+  </si>
+  <si>
+    <t>Франция</t>
+  </si>
+  <si>
+    <t>Апостол от 70-ти</t>
+  </si>
+  <si>
+    <t>03.10/16.10.</t>
+  </si>
+  <si>
+    <t>Епископ, апостол.</t>
+  </si>
+  <si>
+    <t>Дионисий жил в Афинах. Там же он получил классическое эллинское образование.
+Следуя примеру Пифагора и Платона, он отправился в Египет, в город Гелиополь, изучать астрономию. Там вместе со своим другом философом Аполлофаном он стал свидетелем солнечного затмения во время распятия Иисуса Христа (Мф. 27:45). Дионисий воскликнул:
+«Это или Бог, Создатель всего мира, страждет, или этот мир видимый кончается»
+По возвращении в Афины за свою мудрость Дионисий был избран членом Ареопага. Когда в Афинах апостола Павла пригласили в Ареопаг для разъяснения нового учения, Дионисий присутствовал на проповеди и уверовал во Христа (Деян. 17:34). После принятия крещения Дионисий три года провёл возле апостола Павла, после чего был рукоположен в епископа Афинского. В 57 году Дионисий присутствовал при погребении Девы Марии в Иерусалиме.
+В конце 60-х годов I века Ареопагит посещает Рим для свидания с апостолами Петром и Павлом, схваченными императором Нероном. После казни апостолов Дионисий вместе с пресвитером Ру́стиком и диаконом Елевфе́рием отправляется с проповедями в Рим, Германию, Испанию и Францию, продолжать дело апостола Павла. В Лютеции Галлийской, во времена преследования христиан, проповедники были схвачены и брошены в темницу. Правитель Сисиний всех троих осудил за веру, убеждал и мучил, чтобы отреклись они от Христа. Правитель приказал наказать святых мечом. Обезглавленное тело священномученика Дионисия встало, взяло в руки свою голову и пошло к тому месту, где была христианская церковь (около шести километров до поселения, которое впоследствии стало носить имя Сен-Дени).</t>
+  </si>
+  <si>
+    <t>https://azbyka.ru/otechnik/Dmitrij_Rostovskij/zhitija-svjatykh/851</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Дионисий_Ареопагит#/media/Файл:Hosios_Loukas_(diakonikon,_arch)_-_Dionysius_Areopagite.jpg</t>
+  </si>
+  <si>
+    <t>96 г.</t>
+  </si>
+  <si>
+    <t>монастырь Сен-Дени, Париж, Франция</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ерм </t>
+  </si>
+  <si>
+    <t>г. Филиппополь, Болгария</t>
+  </si>
+  <si>
+    <t>05.11./18.11.</t>
+  </si>
+  <si>
+    <t>Римский гражданин, но по происхождению грек. Жил в конце I века. Был епископом в Филиппополе Фракийском. О Ерме упоминается апостолом Павлом в Послании к Римлянам: приветствуйте Асинкрита, Флегонта, Ерма (Рим.16:14).
+Ерм – автор книги «Пастырь», написать которую его побудили откровения свыше. В самом «Пастыре» о его авторе сообщается, что он жил в Риме во время папы Климента, был сначала богат, занимался мирскими делами, имел злоязычную жену и порочных сыновей, к которым не был достаточно строг и за это наказан от Бога потерей богатства. Недоумевая о причинах постигшего его бедствия, Ерм был вразумлен об этом в ряде бывших ему видений. Эти видения и наставления и составляют содержание книги. По форме изложения «Пастырь» принадлежит к числу апокалиптических произведений. Книга имела такое влияние, что временно вносилась, как составная часть, в Библию, но не вошла в окончательный канон Священного Писания.
+Святой апостол от 70 Ерм был епископом в Филиппополе, мученически скончался в I веке. В Послании к Римлянам святой апостол Павел призывал римлян приветствовать апостола Ерма (Рим.16:14).</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Ерма</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Ерма#/media/Файл:Hermes_of_Philippopolis.jpg</t>
+  </si>
+  <si>
+    <t>Григорий Неокесарийский</t>
+  </si>
+  <si>
+    <t>213 г.</t>
+  </si>
+  <si>
+    <t>г. Неокесария, Малая Азия</t>
+  </si>
+  <si>
+    <t>III в.</t>
+  </si>
+  <si>
+    <t>IV в.</t>
+  </si>
+  <si>
+    <t>17.11/30.11.</t>
+  </si>
+  <si>
+    <t>Епископ, богослов</t>
+  </si>
+  <si>
+    <t>Григорий Неокесарийский (Чудотворец) происходил из знаменитой, обеспеченной семьи; являлся потомком греческих поселенцев.
+Точная дата его рождения неизвестна. Считается, что он появился на свет около 213 года, в Неокесарии Понтийской. Согласно преданию, первоначально он именовался Феодором, а имя Григорий, вероятно, получил при Крещении.
+Отец Феодора, далёкий от православного мировоззрения, воспитывал сына, как язычник язычника. Будучи человеком не бедным, он стремился дать ему хорошее светское образование. Между тем, в четырнадцатилетнем возрасте Феодор лишился отца, и многое в предполагавшейся карьере стало зависеть от его близких и от него самого, но главное, от Премудрого Бога.
+Какое-то время Феодор учился в школе грамматика, потом – в школе ритора, затем погрузился в юриспруденцию; готовясь стать адвокатом, изучал законы и право, и, конечно, использовавшийся в то время язык законов – латинский. Желая познать основы римского права, он предполагал было отправиться в Рим. Но по Промыслу Божьему его жизнь сложилась не так, как когда-то задумывал он и язычник-отец.
+Сопроводив в Кесарию сестру, муж которой получил от властей должность советника при наместнике Палестины, Феодор, прибывший туда вместе со своим братом, Афинодором, имел возможность продолжить образование в Берите, где в то время располагалась известная в регионе юридическая школа.
+Но здесь произошло то, о чём никто из близких даже и не предполагал. В тот период в Кесарии Палестинской действовала богословская школа, организованная стараниями знаменитого христианского учителя Оригена. Освоившись по прибытии, Феодор вместе с братом, то ли целенаправленно, то ли из любопытства, захотел услышать проповеди Оригена.
+Вскоре состоялась их встреча (есть мнение, что этому поспособствовал епископ Фирмилиан). Встреча переросла в личное знакомство, которое повлияло на судьбу Феодора самым решительным образом. Феодор, услышав пылкие, красноречивые наставления, проникся к Оригену симпатией и уважением, а Ориген, в свою очередь, предложил взять его к себе в ученики. За Феодором последовал и его брат, Афинодор.
+Поначалу Ориген учил Феодора обнаруживать и собирать семена истины, содержащиеся в философских системах, и вообще приобщил его к любомудрию. Затем он последовательно раскрыл ему смысл Книг Священного Писания, научил доверять Сверхъестественному Откровению и христианскому учению.
+По завершении обучения у Оригена, длившегося, как полагают, не менее пяти лет, Феодор с радостью принял Крещение, публично почтил своего наставника добрым словом и вместе с братом вернулся в родные края.
+Вскоре (Феодор) Григорий получил от Оригена послание, в котором тот настоятельно призывал его направить свои способности, силы и знания на спасение собственной души и на пользу Церкви.
+Пастырское служение
+Обретя в христианстве надёжные нравственные ориентиры, Григорий, по примеру многих великих подвижников, решил уединиться от суеты мира и посвятить свою жизнь служению Тому, Кто Сам в Себе есть Истинная Жизнь.
+Приблизительно в 245 году епископ Амасийский Федим рукоположил его во епископа Неокесарийского. Поначалу Григорий, по смиренному осознанию собственной недостойности, наотрез отказался принять столь высокое звание и достоинство.
+В знак несогласия и нежелания занимать епископскую кафедру, Григорий удалился, но Федим против его несогласия заручился согласием Божьим. Правильно понимая, что Господь равно видит его и Григория, Федим, помолившись, наложил на Григория слово вместо руки и назначил ему в управление город.
+Узнав о случившимся, и, вероятно, почувствовав благодатное озарение, Григорий, конечно же, изумился. Противостоять такому неординарному назначению он не мог, ведь одно дело – возражать Амасийскому епископу, и совсем другое – Господу епископа. После того как Григорий дал своё согласие, его посвятили в архиерея в соответствии с каноном.
+Осуществляя служение, епископ Григорий пользовался у своей паствы чрезвычайно глубоким уважением и авторитетом. Между тем, сила его слова и личного примера оказывала колоссальное воздействие не только на верующих, но и на язычников. Об этом красноречиво свидетельствует зафиксированный в предании факт: к моменту начала его архиерейского служения в городе находилось всего несколько верующих, а под конец, когда он искал, нет ли кого-нибудь ещё, кто бы нуждался в обращении к Искупителю, обнаружилось всего несколько заблудших.
+Слава о Григории перешагнула далеко за границы округи. Жившие позже него святые отцы по праву именовали его Великим, Знаменитым. Как следует из утвердившегося в V веке дополнения к его имени, «Чудотворец», за святость жизни он был удостоен от Бога и дара чудотворений.
+Во время гонения на христианство при Декии святитель Григорий, проявляя благоразумную осторожность, скрывался от язычников вместе со своей паствой в окрестных горах. И Бог хранил его. После прекращения гонения святитель инициировал распространение практики празднований в честь мучеников за Христа.
+В 264 году епископ Григорий принял участие в Антиохийском Поместном Соборе, созванном против еретика Павла Самосатского, ложно учившего о Пресвятой Троице и отрицавшего Божественное достоинство Иисуса Христа.
+Точная дата смерти Григория Чудотворца нам не известна. Полагают, что он почил о Господе в период между 270 и 275 годами.
+Творческое наследие
+Несмотря на богатую проповедническую деятельность святого Григория, количество дошедших до нас письменных поучений (достоверность которых не подвергается сомнению) не велико.
+Среди них особое место занимает обозначаемый его именем Символ (Символ веры Григория Чудотворца, см.: Изложение веры).
+Существует предание, что текст этого краткого изложения догматов веры Григорий получил прежде возведения на Неокесарийскую кафедру. Однажды, когда он пребывал в молитве и богомыслии в безлюдной пустыне, к нему подошли два необычных человека: благообразный старец и светоносная Жена. По слову Жены, её спутник и преподал Григорию Символ, который, впоследствии, он внедрил в Неокесарийской общине. Под явившейся Женой издревле разумеется Богородица, а под старцем – Евангелист Иоанн Богослов.
+Этот символ с ранних времен почитался Церковью как одно из лучших изложений догматов веры.
+Среди прочих творений уместно назвать: Благодарственная речь Оригену, К Татиану краткое слово о душе, К Филагрию о единосущии, К Феопомпу о возможности и невозможности страдания для Бога, Канонические правила Православной Церкви с толкованиями. Правила святых отцов – Каноническое послание святаго Григория Неокесарийскаго 262 г., Подробное изложение веры, Переложение Екклезиаста.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Григорий_Чудотворец</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Григорий_Чудотворец#/media/Файл:Grigorii_chudotvoretz.jpg</t>
+  </si>
+  <si>
+    <t>270 г.</t>
+  </si>
+  <si>
+    <t>Кикилия (Цецилия) Римская</t>
+  </si>
+  <si>
+    <t>Рим, Италия</t>
+  </si>
+  <si>
+    <t>22.11/05.12</t>
+  </si>
+  <si>
+    <t>Святая мученица Кикилия была римлянкой из богатого и знатного рода. Она с юности восприняла христианскую веру и усердно молилась, помогала нуждающимся, под богатой одеждой скрывала власяницу. Родители решили выдать Кикилию замуж за знатного язычника Валериана. Святая не осмелилась перечить воле родителей, но со слезами молилась Богу, чтобы ее жених уверовал во Христа, а она сохранила бы девство. Святая уговорила жениха пойти с ней к епископу Урбану, скрывавшемуся от гонений в пещере у Аппиевой дороги. Наставления мудрого старца проникли в душу Валериана, и он уверовал во Христа и обратил в христианство и своего брата Тивуртия. Братья роздали часть своего имения бедным, ухаживали за больными, хоронили христиан, замученных гонителями.
+Правитель Аммах, узнав об этом, повелел схватить братьев и привести на суд. Он потребовал, чтобы святые отреклись от Христа и принесли жертвы языческим богам. Братья отказались. Тогда мучеников стали беспощадно избивать плетьми. Святой Валериан под пытками убеждал христиан не пугаться мук, но твердо стоять за Христа.
+Правитель, желая избежать влияния святого проповедника на народ, приказал вывести мучеников за пределы города и там казнить. Отрядом воинов, сопровождавших мучеников на казнь, командовал Максим. Его поразило мужество святых. Он спросил, почему они не боятся смерти. Святые братья ответили, что они оставляют временную жизнь ради жизни вечной. Максим захотел подробно узнать учение христиан. Он привел святых Валериана и Тивуртия в свой дом и всю ночь слушал их беседу. Узнав об этом, святая Кикилия пришла к Максиму со священником, и он со всей семьей принял Святое Крещение.
+Когда на следующий день мучеников Валериана и Тивуртия обезглавили, святой Максим всенародно исповедал, что он видел, как их святые души восходили к Небесам. За это исповедание святой мученик Максим был насмерть забит плетьми († 230).
+Правитель хотел завладеть имением казненных, но, узнав, что святая Кикилия уже раздала все оставшееся имущество нищим и своей проповедью обратила в христианство 400 человек, приказал казнить ее. Три дня ее морили жаром и дымом в накаленной бане, но благодать Божия хранила ее. Тогда ее решили обезглавить. Палач ударил мечом святую, но лишь ранил ее. Святая мученица страдала еще три дня в полном сознании, утверждая в вере окружающих, и скончалась с молитвой на устах.</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Цецилия_Римская</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Saint_Cecilia#/media/File:Franciscan-Sisters-Saint-Cecilia-window-vocations-fscc-calledtobe.org.jpg</t>
+  </si>
+  <si>
+    <t>230 г.</t>
+  </si>
+  <si>
+    <t>Григорий Богослов</t>
+  </si>
+  <si>
+    <t>330 г.</t>
+  </si>
+  <si>
+    <t>г. Назианз, Каппадокия, Малая Азия</t>
+  </si>
+  <si>
+    <t>г.Константинополь</t>
+  </si>
+  <si>
+    <t>30.01/12.02</t>
+  </si>
+  <si>
+    <t>Епископ, богослов.</t>
+  </si>
+  <si>
+    <t>Святитель Григорий Богослов родился в юго-западной области Каппадокии, в Арианзе (недалеко от города Назианза), приблизительно около 330 года.
+Происходил он в прямом смысле этого слова из семьи святых: отец – Григорий, епископ Назианзский, мать Нонна, брат Кесарий и сестра Горгония – все они после своей кончины были канонизированы.
+Его родной отец, Григорий старший, в свое время он принадлежал к сторонникам культа, поклонявшихся Богу как Высочайшему, но при этом исповедовавших веру, состоящую из смеси положений христианства, иудейства и персидских учений. Ко Христу он обратился по молитвам супруги, Нонны, глубоко верующей, ревностной христианки. Под её благотворным влиянием он принял Крещение. Вскоре его посвятили во священника, а впоследствии возвели на епископскую кафедру в Назианзе.
+Ещё до появления на свет Григория младшего, будущего святителя Григория Богослова, Нонна усердно молилась Богу о даровании ей сына и обязалась, что в случае, если её молитва будет исполнена, она посвятит дитя Богу. Сын был дарован, обещание исполнено.
+С детских лет Григорий младший воспитывался в любви к Богу и ближним. Первоначальное образование, в том числе в области основ Православного вероучения, он приобрёл в родительском доме. Благодаря влиянию матери он ещё с юности определился, что будет вести безбрачную, богоугодную жизнь.
+По мере взросления, он проходил обучение в лучших для той поры школах: в Кесарии Каппадокийской, в Кесарии Палестинской, в Александрии, в Афинах. Обучение обходилось недешево, но материальное состояние родителей это позволяло.
+В Кесарии Каппадокийской Григорий познакомился с будущим вселенским учителем, святителем Василием Великим. Затем их знакомство продолжилось во время учёбы в Афинах и переросло в крепкую дружбу.
+Возвратившись из Афин (приблизительно в 358 году), Григорий принял Крещение, после чего предался аскетической жизни: проводил жизнь в постах, молитве, богомыслии и созерцании. В этот период он посещал Понт, ища встреч и совместных подвигов со своим другом и единомышленником Василием. Одним из плодов их творческого сотрудничества стало произведение «Филокалия», включавшее мысли и выдержки из сочинений знаменитого церковного учителя Оригена.
+Около 360 года Григорий старший, отец Григория Богослова, не вполне понимая тонкости распространившегося к тому времени арианского лжеучения, подписал арианский символ, чем вызвал негодование православных, представителей его паствы. Многие готовы были отойти от своего епископа. В тот момент Григорий младший сумел разъяснить отцу его ошибку и показать несоответствие подписанного Символа Никейскому. В результате Григорий старший признал заблуждение публично и порядок среди его паствы был восстановлен.
+Священническое и епископское служение
+В 361 году, в день торжественного празднования Рождества Спасителя, Григория, вопреки его возражениям, рукоположили во священника. По смирению он был против этого посвящения, но опять же, по смирению не решился противиться воле архиерея, отца. Опечалившись таким поворотом событий, Григорий отправился в Понт, к Василию. Тот сумел подобрать нужные слова утешения и ободрил давнего друга.
+К Пасхе 362 года отец Григорий возвратился в Назианз и приступил к деятельному исполнению пастырского долга. С того времени он находился при вверенной ему пастве и по мере возможностей помогал родному отцу, Григорию старшему, в его архиерейском служении.
+Когда в 370 году Василия Великого возвели в архиепископа Кесарийского, тот, в целях лучшего управления своей паствой и борьбы с арианством, стал открывать новые кафедры. В этот период он нуждался в ревностных, религиозно-образованных пастырях.
+Следуя своему замыслу святитель Василий поставил своего друга, Григория, епископом в Сасим. Шёл 372 год. Григорий Богослов хотя и понимал, в чём состояла важность этого шага с позиции Василия Великого, и согласился, однако, как и в случае с рукоположением во священника, подчинился этому выбору с неохотой, а затем удалился в безлюдное, пустынное место, где предался созерцательной молитве.
+Через какое-то время Григорий старший уговорил своего сына прибыть в Назианз. Тот вернулся, но с условием, что не будет преемником по кафедре отцу.
+В 374 году умер отец Григория Богослова, а вскоре и мать. Придя в храм, где служил и её супруг, и её любящий сын, и приблизившись к жертвеннику, она внезапно почувствовала приближение смерти, произнесла молитву и предала душу Богу. Всё это, конечно же, отразилось на внутреннем состоянии Григория. Какое-то время он продолжал дело отца, но вскоре заболел, да так тяжело, что некоторые даже и не надеялись на его выздоровление.
+В 375 году, оправившись от недуга, желая предаться уединённому жительству, он удалился в Селевкию Исаврийскую. Здесь он жил так, словно бы сам себя заточил. Страшное огорчение принесла ему весть о смерти Василия Великого (379 г.).
+Борьба с ересью. Литературная деятельность
+После смерти Валента, покровительствовавшего арианским «священнослужителям», на царский трон взошёл Феодосий, который поддерживал православных.
+В 379 году верующие граждане Константинополя обратились к святителю Григорию с призывом о помощи. Внявший советам друзей и чувству пастырского долга, он оставил уединение и поспешил в столицу.
+Увиденное там привело его в состояние праведного негодования: храмы были захвачены арианами, внутри православных отсутствовало единство, нравы жителей отличались распущенностью и развращенностью. Святитель Григорий вынужден был искать себе более или менее безопасное пристанище и обрёл его в частном доме.
+Ревность о Господе, преданность Православию, трезвомыслие, образованность и, конечно же, красноречие Григория Богослова не могли не вызвать надлежащего отклика в сердцах горожан. Под действием его увещеваний и проповедей люди преображались. Многие пламенели желанием увидеть и послушать ревностного защитника веры. Очень быстро слава святителя достигла такого размаха, что стала привлекать в Константинополь даже и жителей отдаленных селений.
+Всё это вкупе возбуждало у последователей Ария недружелюбные, агресивные чувства. Еретики были готовы не только интриговать против святителя, но даже и покушались на его жизнь.
+Прибывший в 380 году в Константинополь государь, Феодосий, прибегнул к возможностям своей, царской, власти и передал захваченные еретиками храмы в руки Православных. Святитель Григорий, понимая необходимость личного присутствия, согласился остаться в столице, пока не соберется намеченный Собор.
+Деятельность святителя Григория на Константинопольском Соборе
+Именно этому Собору, состоявшемуся в 381 году, получившему статус Второго Вселенского, надлежало поставить заключительную точку в догматических спорах ариан с Православными, что и было исполнено.
+На Соборе присутствовали такие выдающиеся отцы Церкви как Мелетий Антиохийский, Григорий Нисский и др. Учитывая желания императора, большинства духовенства и простых верующих, святитель Григорий был избран на Константинопольскую Патриаршую кафедру, а после смерти Мелетия Антиохийского его провозгласили председателем Собора.
+Но здесь в дело вмешались прибывшие на Собор египетские архиереи, желавшие видеть на Патриаршем престоле своего ставленника. Возбудили полемику, нашёлся и подходящий мотив: ссылаясь на каноническое правило Никейского Собора, запрещающее переход епископа с одной кафедры на другую, объявили поставление святителя Григория в епископа Константинопольского незаконным.
+Несмотря на то, что действие канона, принятого отцами Первого Вселенского Собора, было перекрыто самим избранием святителя Григория отцами Второго Вселенского Собора, за этот формальный предлог уцепились. Как только сформировалась удобная почва для развития интриги, против Григория стали высказываться как те, кто питали к нему недовольство за снисходительность в отношении ариан (как заблудших людей), так и те, кто не желали мириться с его строгостью в деле борьбы за чистоту веры.
+Святитель Григорий, чуждый почестей, а тем более гнусных интриг, счёл за лучшее отказаться от полномочий предстоятеля Константинопольской Церкви и удалиться из города. Перед отбытием он произнёс пред собравшимися прощальную речь, в рамках которой изложил свою христианскую позицию и раскрыл свою пастырскую правоту.
+Последний период земной жизни
+Некоторое время спустя Григорий Богослов прибыл в Назианз, возглавил там местную паству и руководил ею вплоть до момента, когда на кафедру Назианза взошёл епископ Евлавий. Произошло это в 383 году.
+После сего святитель переселился на малую родину, в Арианз, где предался молитвенному созерцанию и писательской деятельности.
+В 389 году он мирно почил о Господе.
+За святость и праведность жизни, яркое, безукоризненное изложение в своих сочинениях учения о Пресвятой Троице и Лице Господа Иисуса Христа Вселенская Православная Церковь почтила его исключительным по значению именем – Богослов. С этим именем в Историю Церкви вошли всего три святых; помимо свт. Григория – апостол Иоанн Богослов и Симеон Новый Богослов. 
+Святитель Григорий Богослов оставил после себя богатое литературное наследие, состоящее из 245 писем, 507 стихотворений (написанных подчас в подражании Гомеру в формах гекзаметров, пентаметров, триметров) и 45 «Слов».</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Григорий_Богослов</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Григорий_Богослов#/media/Файл:Sv_Gr_Bogoslov_Simonopetra_kr18v.jpg</t>
+  </si>
+  <si>
+    <t>389 г.</t>
+  </si>
+  <si>
+    <t>г. Константинополь</t>
+  </si>
+  <si>
+    <t>Николай Мирликийский</t>
+  </si>
+  <si>
+    <t>г. Патара, Малая Азия</t>
+  </si>
+  <si>
+    <t>г. Миры Ликийские, Малая Азия</t>
+  </si>
+  <si>
+    <t>г. Никея, Малая Азия</t>
+  </si>
+  <si>
+    <t>06.12./19.12.; 09.05./22.05.</t>
+  </si>
+  <si>
+    <t>Отчизной иерарха Христова Николая(*) был древний ликийский[2] город Патара[3]. Его родители происходили из знатного и богатого рода, но никогда не стремились к мирской славе и роскоши. Они весьма выделялись среди соотечественников своими добродетелями[4]. За богоугодную жизнь супруги удостоились высокой чести стать святым корнем, произрастившим древо чудоточное рая Иисусова(*). Словно дерево, посаженное при потоках вод, которое приносит плод свой во время свое (Пс.1:3), у благословенной четы как плод праведности родился великий заступник вселенной Николай[5].
+С первых дней жизни младенца его поведение было необычным: во время кормления Николай сосал молоко только из правой груди матери, а по средам и пятницам вкушал лишь один раз, и то вечером, в девятом часу(*). Это знамение предопределило весь образ жизни Николая. Так, от младенческих пелен до самой кончины святой проводил среду и пятницу в строгом посте и воздержании.
+Николай был единственным ребенком в семье. Родители[6] сами ухаживали за ним, очень любили и оберегали свое дитя. Добронравие младенца восхищало их – супруги считали себя счастливейшими из людей. Они, не жалея сил, старались совершенствовать прекрасные от природы свойства его души. Благословенная чета свято соблюдала заповеди Господни, показывая сыну дивный пример нестяжания и праведности.
+Когда мальчик подрос, родители отдали его учиться[7]. Благодаря природным дарованиям и остроте ума Николай преуспел в изучении многих наук(*), а действием благодати Святого Духа в совершенстве постиг премудрость Божественного Писания. В стремлении к духовному возрастанию юноша не ограничился только книжным образованием, но показал себя совершенным и в самой жизни.
+Николай во всем следовал наставлениям богобоязненных родителей. Он избегал пустых, суетных развлечений толпы, несовместимых с добродетельной жизнью, всячески уклонялся от непристойных бесед с праздными юношами и навсегда удалил из своего сердца любовь к театральным зрелищам(*). Святой хранил непорочным целомудрие, дабы душегубительная страсть к женщинам не овладела умом и не запятнала его мужественной праведности. Николай стремился проводить дни и ночи в богомыслии и созерцании Господа, прилежно собирая мед добродетелей. Будущий святитель усердно посещал церковь. Там он приобщался благодати Святого Духа и созидал в себе достойное для Него жилище, по слову Писания: вы храм Божий, и Дух Божий живет в вас (1Кор.3:16).
+Святой Дух поистине обитал в этом благоговейном и чистом юноше, сохранившем неугасимым светильник девства. Служа Господу, он пламенел любовью к Нему. За Николаем не замечалось никаких привычек, свойственных молодости. По своему нраву молодой праведник был подобен старцу – все уважали его и удивлялись ему. Когда старый человек выказывает юношеские увлечения, он для всех служит посмешищем, а если юноша имеет нрав старца, то вызывает всеобщее уважение. В старости неуместно легкомыслие юности, но достойна почтения и прекрасна в юноше мудрость старца.
+Епископ(*) города Патары видел, что Николай преуспевает в добродетельном житии и устраняется от всего мирского. Архиерей рукоположил избранника Божьего в клирики[8].
+Теперь усердный хранитель чистоты Николай стал вести еще более строгую подвижническую жизнь. Приготовляя себя для благоугождения Вечному Царю, святой уподобился бесплотным: он бодрствовал и пребывал в непрестанной молитве и посте. Наделенный всеми дарами Божьими, юный клирик день ото дня расцветал красотой равноангельской жизни.
+Посвятив себя Господу, Николай продолжал усердно заботиться об отце и матери и не расставался с ними до самой их кончины. Его родители встретили смерть с надеждой на милость Отца Небесного благодаря великой славе светоча Христова Николая. Так и случилось. За своего ангелоподобного сына они и Богу угодны, и у людей имеют присноблаженную память в веках.
+После смерти родителей Николай получил большое наследство. Но блестящее состояние не приносило ему радости. Боголюбивый юноша не дорожил скоропреходящим богатством и не заботился о его приумножении, ибо знал: Доброе имя лучше большого богатства, а добрая слава лучше серебра и золота (Притч.22:21). Святой стремился собрать нетленные сокровища в нерасхищаемых небесных кладовых. Щедрая рука Николая была простерта к нуждающимся людям и словно многоводная река изливала на них обильную милостыню. Отрекшись от всяких мирских желаний, сердобольный юноша попросил Бога указать ему, как наилучшим образом раздать наследство бедным: К Тебе, Господи, возношу душу мою. Научи меня исполнять волю Твою, потому что Ты Бог мой (Пс.24:1, 142:10).
+Вот одно из многих дел его милосердия.
+В городе Патара в доме по соседству с блаженным Николаем жил знатный и очень богатый человек[9]. Он имел трех дочерей, отличавшихся необычайной красотой. Вследствие неблагоприятных обстоятельств этот богач разорился и потерял прежнее влияние, ибо жизнь века сего непостоянна. Несчастный отец не смог выдать девушек замуж, так как женихи стали гнушаться их крайней бедностью. Постепенно сосед Николая впал в нищету – его семье нечего было есть и не во что одеться. Тогда он задумал превратить свое жилище в дом блуда, отдав дочерей на любодеяние, и таким образом добыть средства к существованию.
+О, горе! До чего только нищета не доводит человека, который отчаялся в уповании на Бога! Уже хотел малодушный отец исполнить свое злое намерение, но Всевидящий Господь подал благую мысль Николаю спасти разорившееся семейство.
+Посмотри же, читатель, на доброту души человеколюбивого Николая и сам стань истинным подражателем его милосердия, дабы и тебе быть помилованным по заповеди Христа: Блаженны милостивые, ибо они помилованы будут (Мф.5:7). Мы должны помогать бедным, делая это во славу нашего Творца и Создателя, чтобы святилось в нас Его Имя.
+Великодушный юноша глубоко сострадал нуждающимся людям и извлек отца и его дочерей из нищеты и греха, словно из огня. Однако святой совершил свое благодеяние не открыто, а подал щедрую милостыню тайно. Николай поступил так по двум причинам. Прежде всего он сам хотел избежать суетной славы, следуя словам Евангелия: Смотрите, не творите милостыни вашей пред людьми с тем, чтобы они видели вас (Мф.6:1); с другой стороны, боялся уязвить самолюбие мужа, еще недавно обладавшего большим состоянием. Святой понимал, как сильно можно унизить подаянием человека, который от богатства и славы пришел к нищете.
+Николай ночью незаметно бросил полный узелок с золотом(*) в окно соседа и быстро удалился. Можно себе представить несказанную радость отчаявшегося мужа, когда он утром нашел в своем доме то, из-за чего хотел подвергнуть позору дочерей.
+Отец не верил своим глазам, удивлялся и недоумевал, не сон ли это. Пощупав деньги, бедняк убедился, что держит в руках золотые монеты, и заплакал от счастья. Он долго размышлял, кто из друзей мог послать ему столь драгоценный дар. Перебрав в памяти всех знакомых, спасенный от пагубного грехопадения муж понял – только Промысл Божий мог даровать его семье тайного благодетеля. Тогда отец разоренной семьи возблагодарил Господа и отдал золото старшей дочери в приданое.
+После ее свадьбы сердобольный Николай, видя, как его подаяние уберегло от погибели старшую сестру, позаботился и о средней дочери. Тайно от всех, ночью, добрый юноша снова бросил узелок в окно соседа. Утром хозяин дома нашел золото. Обливаясь слезами, он пал ниц и произнес:
+– Боже Всемогущий, покажи мне слугу Твоего безмерного человеколюбия. Покажи мне этого земного ангела, дабы я мог узнать, кто спасает мой дом от угнетающей нищеты и избавляет нас от греховных мыслей и намерений. Господи, по Твоей милости, тайно творимой щедрой рукой неизвестного мне Твоего угодника, я смогу отдать замуж вторую дочь и тем избежать сетей дьявола, который хотел погубить мою семью.
+Бедняк горячо поблагодарил Бога за Его дивное попечение о нем и отпраздновал свадьбу второй дочери. Теперь сосед Николая уже твердо надеялся, что Господь подаст той же благодетельной рукой приданое на законный брак и для младшей дочери. Дабы узнать, кто приносит в дом золото, он не спал ночи в ожидании своего покровителя. Прошло немного времени. Глубокой ночью Николай тихо пришел в третий раз, остановился на обычном месте, бросил в окно узелок и тотчас поспешил уйти. Услышав звон золота, хозяин быстро побежал вслед за угодником Божьим и догнал его. Бедняк сразу узнал в нем соседа, припал к стопам святого, целовал их и называл Николая избавителем, помощником и спасителем семьи, оказавшейся на краю погибели.
+– Если бы, – говорил он, – Великий в Своем милосердии Господь не послал мне твоими руками изрядную помощь, то я погиб бы вместе с дочерьми в адском огне. Ныне же мы спасены тобой и избавлены от ужасного грехопадения.
+Еще много благодарственных слов произнес счастливый муж со слезами радости. Николай поднял соседа с земли и попросил никому не открывать его имени[10]. Святой дал полезные наставления отцу спасенной им семьи и отпустил его с миром.
+Мы поведали читателю лишь об одном из дел милосердия святого Николая в Патаре, но в древних текстах сообщается[11], что невозможно даже кратко рассказать, сколько голодных он накормил в родном городе, сколько одел нагих, сколько выкупил должников.
+Святой избегал земной славы и пытался скрывать от людей свои добрые дела, но Бог, прославляющий славящих Его (ср. 1Цар.2:30), пожелал открыть для всех это многоценное сокровище добродетелей, которым Он решил обогатить мир. Молва о щедрости и милосердии к бедным молодого клирика распространилась по городу. Архиерей по достоинству оценил сияющего целомудрием юношу: владыка рукоположил Николая в пресвитеры и по внушению Святого Духа пророчески сказал народу в церкви:
+– Братья! Я вижу новое солнце, восходящее над землей. Блаженно то стадо, которое удостоится иметь его своим пастырем, ибо он упасет души заблудших, насытит их на пажити благочестия и явится милосердным помощником в бедах и скорбях.
+Преподобный Николай, как мы уже знаем, с младенческих лет посвятил свою жизнь благоугождению Богу. Научившись подчинять разуму чувства и желания, усердный подвижник стал превыше страстей и греха. Добродетели пастыря не остались в тени – люди начали почитать Николая за его смиренномудрие и восхищались стойким нравом этого человека. Множество народа стекалось к святому, и все получали от него утешение и помощь. И он пас их в чистоте сердца своего и руками мудрыми водил их (Пс.77:71-72)[12].
+Вскоре Господь приготовил великому светочу достойную лампаду. Вседержителю было угодно возвести пресвитера Николая в архиерейское достоинство, дабы он, соединив власть со справедливостью, мог защитить ликийскую паству от козней видимых и невидимых врагов.
+Смотрение Божье мудро устраивает жизнь святого – Господь привел Николая в Миры[13], главный город митрополии, как раз в то время, когда скончался предстоятель Ликийской Церкви.
+Духовенство и народ находились под влиянием удивительной богоугодной жизни почившего архиепископа. Они хотели избрать на его место человека, не уступающего прежнему владыке в святости и заботе о делах митрополии. Движимый Божественной ревностью, один архиерей предложил собравшемуся духовенству обратиться за помощью ко Господу:
+– Избрание епископа на престол – дело Божьего устроения. Нам подобает совершить молитву, а Господь Сам откроет, кто достоин стать предстоятелем нашей митрополии.
+Мудрый совет встретил всеобщее одобрение. Единодушие было полным, словно каждый и ранее держался этой мысли. Господь внял их усердной молитве, и в ночном видении Голос свыше повелел одному из участников собора:
+– Отправься рано утром в храм и встань в притворе. Кто первым придет в церковь, тот и есть Мой избранник; примите его с честью и поставьте в архиепископы – имя этого мужа Николай.
+О Божественном повелении архиерей сообщил епископам и клирикам, и они усилили молитвы. Владыка, удостоившийся откровения, стал ожидать желанного мужа в притворе храма.
+На рассвете, после ударов в било, прежде всех пришел в церковь подвигнутый Духом Святым богоблаженный Николай. Как только он появился у двери храма, архиерей остановил его и спросил:
+– Чадо, как твое имя?
+Святой кротко ответил епископу:
+– Имя мое Николай, я раб твоей святости, владыка.
+Благочестивейшего архипастыря поразил смиренный ответ праведника. Он уразумел, что перед ним тот самый муж, которого Бог хочет поставить во главе Ликийской Церкви, ибо знал: Господь благоволит к человеку кроткому и смиренному. Велика была радость владыки, когда ему открылось тайное сокровище. Тотчас со словами: «Следуй за мною, чадо» – архиерей торжественно привел святого к епископам, которые с радостью приняли его. Молва о предуказании Божьем быстро разнеслась по городу, и в церкви собралось множество народа. Епископы вывели Николая на середину храма, чтобы показать людям пастыря, посланного Господом. Владыка, удостоившийся видения, воскликнул:
+– Вот, братья, муж, избранный Богом предстоятелем Христовой Церкви в Ликии. Не человеческой волей поставлен он над нами, но Сам Дух Святой вверил ему попечение о душах наших. Под его управлением и мудрыми наставлениями не страшно будет нам предстать перед Богом в день Второго пришествия Христова.
+Народ с неизреченной радостью слушал владыку и горячо благодарил Господа(*).
+Преподобный Николай избегал мирской славы. Обладая воистину достохвальной скромностью, он сначала отказался принять архиерейский сан. Но когда святой узнал об откровении свыше, то усмотрел в видении явное изволение Божье на избрание и уступил усердным мольбам духовенства и народа.
+Собор епископов совершил хиротонию над пресвитером Николаем, и все светло праздновали обретение дарованного Господом иерарха(*). Так по справедливому Божьему выбору всеблаженный Николай стал главой славной Мирликийской митрополии и воссиял для Христовой Церкви светом веры и благочестия. С тех пор он озаряет спящих в ночи неведения ничуть не менее ярчайшего солнца, восходящего над океаном.
+В самом начале архиерейского служения угодник Божий так говорил себе:
+– Николай! Принятый тобой святительский сан требует от тебя иного образа жизни: отныне ты должен жить не только ради своего спасения, но прежде всего – для спасения других.
+Желая научить паству благочестию, он не скрывал уже, как раньше, свое добродетельное житие. Теперь его жизнь стала открыта для всех, но не ради тщеславия перед людьми, а для их пользы и умножения славы Божьей, во исполнение слов Спасителя: Так да светит свет ваш пред людьми, чтобы они видели ваши добрые дела и прославляли Отца вашего Небесного (Мф.5:16). Добрыми делами святитель Николай воистину стал образцом для верных в слове, в житии, в любви, в духе, в вере, в чистоте (1 Тим 4. 12).
+Вскоре после избрания предстоятелем митрополии Николай Мирликийский созвал Поместный Собор, на котором шла речь о положении клира и всей Церкви. Собор принял ряд мудрых постановлений и созывался святителем ежегодно в первый день сентября[14].
+Архиепископ Николай был кроток нравом, незлобив и смирен духом. Он одевался очень просто и скромно – в одеждах иерарха не было никаких украшений. Поведение владыки отличалось высшей сдержанностью и строгостью[15]. По древнему преданию, богоблаженный Николай имел ангельский лик, исполненный святости и благодати. От него исходило некое пресветлое сияние, как от лица пророка Божьего Моисея[16].
+Став архиереем, он продолжал питаться только постной пищей один раз в сутки, и то вечером. В течение всей жизни владыка не ел мяса[17]. Ужин святителя часто прерывался или отменялся из-за его привычки быть доступным людям, нуждающимся в помощи и совете.
+Весь день святой проводил в трудах и молитвах, но двери его дома не закрывались ни для кого – он всегда выслушивал просьбы людей и помогал им. Владыка для всех стал великим благодетелем: сиротам – отец, нищим – милостивый податель, плачущим – утешитель, обиженным – защитник. Таковы были первые деяния святителя Николая, таковы первые знаки его архипастырского посоха.
+Но завистливое око дьявола не может спокойно смотреть на процветание благочестия. Враг рода человеческого всегда старается причинить вред Христовой Церкви. И на этот раз он не оставил ее в покое. Злой демон вселился в царей, державших скипетр Римской империи, и началось яростное гонение на Церковь: повсюду были разосланы указы императоров Диоклетиана и Максимиана(*) предписывающие христианам отречься от веры в Единого Бога и поклониться идолам. Всех не желающих повиноваться ожидали оковы, темницы, страшные пытки и, наконец, лютая смерть. Эта дышащая злобой буря вскоре достигла города Миры.
+Несмотря на гонения, архиепископ Николай продолжал дерзновенно исповедовать Истинного Бога и был готов пострадать за Христа. За это первые люди города приказали схватить святителя и бросить в тюрьму. Нечестивые мучители приговорили верного служителя Божьего к оковам, дыбе и другим пыткам[18]. Святой Николай довольно долго пробыл в темнице[19]. Вместе с другими христианами он мужественно претерпевал тяжкие страдания, голод, жажду и тюремную тесноту. Святитель переносил тяготы заточения с таким достоинством, с каким другой человек принимает вещи отрадные и желанные. Блаженный Николай совершил подвиг, равный его предшественникам – святым мученикам Крискенту, Диоскориду и Никоклу[20]. Как и они, ревностью о Христе святитель украсил себя мученическим венцом!
+Славный пастырь поил темничных соузников водами благочестия и питал словом Божьим. Многие из заключенных до конца были твердыми в исповедании веры, страдали и умирали за истину, вдохновленные наставлениями богомудрого Николая. Самого же святителя Господь сохранил во время Диоклетианова гонения, ибо дивному избраннику Христову за его деяния и чудотворения предстояло стать великим столпом Церкви, светилом, озарившим всю вселенную лучами добродетелей.
+Убедившись, что жестокость по отношению к христианам не приводит к желанным результатам, император Максимиан оказал им снисхождение и даровал некоторую свободу[21]. Святой Николай был освобожден из темницы(*). Город Миры встретил его как мученика, принявшего бескровный венец[22], а святитель, нося в себе Божественную благодать, снова стал исцелять людей от страстей и недугов. Ликийцы прославляли блаженного Николая, дивились ему, и все любили своего архипастыря, ибо он сиял чистотой сердца, служа Господу в святости и правде пред Ним, во все дни жизни (Лк.1:75).
+Но не раз еще возобновлялись гонения на христиан в восточной части империи, до той поры пока с помощью Божьей равноапостольный царь Константин одержал окончательную победу над соправителем Ликинием, ибо человеколюбивый Бог, взирая с небес, сокрушает и губит все скипетры нечестия. Только тогда для всех христиан наступила тишь после ненастья и воссияло солнце.
+Мудрый царь знал, Кто даровал ему власть над всей Римской державой. После победы над Ликинием он повелел и на Востоке империи освободить из тюрем заключенных там христиан, вернуть им храмы и церковное имущество. Епископ Кесарийский Евсевий Памфил писал: «У нас, возлагавших свою надежду на Христа, Сына Божьего, радость была несказанная; каждое место, еще недавно опустошенное нечестием тиранов, дышало дивным ликованием, словно оживая после длительной смертельной заразы; мы видели, как от основания поднимались церкви, возносясь на недосягаемую высоту в красоте большей, чем у церквей, разрушенных прежде»(*).
+В Мирах, как и в других городах Римской империи, оставалось много языческих святилищ(*). Часть горожан на свою погибель продолжала посещать их и приносить жертвы идолам. Почитание ликийцами ложных богов сильно огорчало архиепископа Николая. Во время правления императоров-язычников, конечно, не могло быть и речи об уничтожении богопротивных капищ. Но теперь, пользуясь благоволением к Христовой Церкви Константина Великого, архиерей Бога Вышнего стал разрушать идольские храмы[23] и очищать город от языческой скверны.
+Так, воюя с духами зла, всеславный иерарх пришел в святилище Артемиды[24]. Это величественное сооружение красотой и размерами превосходило все остальные и было любимым прибежищем демонов. Ревностный защитник благочестия Николай разрушил храм Артемиды до самого основания. Лукавые духи, испуская вопли, бежали из своего жилища, побежденные молитвенным оружием воина Христова Николая.
+В годы царствования боголюбивого императора Константина враг рода человеческого лишился господства над множеством суеверных язычников, но не прекратил злокозненных нападений на Церковь, сея плевелы ересей, которые быстро возрастали и приводили к разногласиям, раздиравшим Христову Церковь. Нетвердые в вере пастыри предавались умствованиям, а неправые умствования отдаляют от Бога (Прем.1:3). Они стали виновниками распространения ложных учений.
+Особенно опасным оказался раскол, порожденный Арием. Эта пагубная ересь, арианство, стремительно расползалась повсюду и вводила многих христиан в заблуждение. Церковь благочестиво учила, что у Святой Троицы Ипостаси одной природы и одной сущности, и Сын и Святой Дух равны Отцу. Она провозглашала три Ипостаси равносильными и равнобожественными, не сливая и не смешивая их, но и не разделяя на три чужеродные. Однако ариане утверждали, что Христос – меньший Бог, чем Бог Отец, и имеет иную сущность, а Святой Дух подчинен Им.
+Ликийская митрополия благодаря бдительному попечению великого наставника Николая не подпустила к себе эту порчу, отбросив ее, как смертоносный яд.
+Огненной проповедью святитель, словно мечом, с корнем отсекал воинственный Ариев раскол вместе с савеллианской и другими ересями. Исповедник Христа Николай считал слово Божье первым и самым действенным средством для обращения еретиков. Святитель Андрей Критский повествует(*), как архиепископ Николай вразумил одного из отступников. Однажды заботливый пастырь, осматривая лозы винограда Христова, встретил маркионитского епископа Феогния. Богомудрый Николай словами Священного Писания изобличал заблуждения маркионитов до тех пор, пока не обратил владыку к истине. Феогний отрекся от ереси, но его самолюбие было ущемлено. Великодушный иерарх заметил, что епископ сильно раздражен, и, возвысив голос, произнес:
+– Солнце да не зайдет во гневе вашем (Еф.4:26). Брат мой! Помиримся.
+Кротостью и смирением архиерей Божий Николай обратил к православной вере епископа Феогния и многих других отступников. Но он мог быть и грозным, если еретик, упорствуя в заблуждениях, оскорблял Господа нашего Иисуса Христа, как это случилось на Соборе в Никее[25].
+Святой равноапостольный император Константин, желая водворить в Церкви мир, повелел созвать в 325 году Вселенский Собор. Архиепископ Николай, как глава Ликийской митрополии, непременно должен был участвовать в его работе(*).
+На Соборе святые отцы[26] изложили незыблемые основы православной веры и предали проклятию арианскую ересь. Многие из них утверждали Православие силой своего просвещения, а Николай защищал веру самой верой: он говорил, что христиане начиная от апостолов неизменно веровали в Божество Иисуса Христа и никогда не принижали Его Ипостась. Святитель прославился на Соборе особым рвением по искоренению ересей и утверждению православной веры. За это Церковь называет его «великим благочестия столпом, твердым православия укреплением, мечом, плевелы прелести посекающим»(*).
+Один из иноков Студийского монастыря повествует о дерзновенном поступке на Соборе верного служителя Христова[27]:
+– На заседании Собора Николай, воодушевленный ревностью о Господе, не стерпев арианского богохульства, ударил еретика по щеке. Отцы сочли дерзким этот поступок. Николай был лишен архиерейского сана и заключен в темницу[28].
+Но Сам Христос и Пресвятая Богородица одобрили Божественную ревность славного поборника истины[29]. Они явились в темницу и вручили ему Евангелие и святительский омофор. В это же время несколько отцов Собора удостоились дивного видения. Владыки узрели заключенного в тюрьму Николая. С левой стороны от блаженного узника стоял Спаситель, подающий ему Евангелие, а с правой – Богородица, возлагающая на него святительский омофор. Архиереи отправились в темницу и увидели Николая, облаченного в омофор, с Евангелием в руке. Отцы Собора поняли, что дерзновение мужественного иерарха было угодно Богу. Святого немедленно освободили из заключения, возвратили ему архиерейский сан и воздали почести как угоднику Божьему.
+По окончании Собора святитель вернулся к своей пастве и преподал всему народу принятый в Никее Символ православной веры. В Ликии верный служитель Живоначальной Троицы пресек в самом корне еретические умствования, а упорствующих еретиков прогнал. Благоразумный земледелец отбирает лучшие зерна и выбрасывает сорняки. Так мудрый Николай – сеятель на ниве Христовой – наполнял духовную житницу плодами добродетелей, плевелы же еретической прелести далеко отметал от пшеницы Господней. Поэтому Церковь называет его «лопатой, развевающей Ариевы плевельные учения»(*).
+Добрый пастырь Христов имел великое попечение о своем отечестве. Он не только духовно окормлял Ликию, но всегда незамедлительно приходил на помощь и спасал ее от, казалось бы, неминуемой беды. По милости Божьей сохранились древние рукописные повествования о деянии святителя, защитившего свою паству от несправедливой подати[30].
+Ныне поведаем читателю об этом пречудном деянии, дабы напомнить, на кого надо уповать и к кому обращаться, когда народ разоряется и голодает от непосильного бремени налогов.
+Император Константин, став единовластным правителем всей Римской державы, решил воздвигнуть новую христианскую столицу – величественный город Константинополь(*). Осуществление благочестивого замысла Василевса потребовало огромных средств. Поскольку подошел срок очередной переписи населения и земельных наделов, во все провинции были посланы переписчики для повышения налоговых сборов(*). В Миры также прибыл царский чиновник. Этот человек оказался хитрым и лживым; он из чувства неприязни к ликийцам и желания выслужиться перед монархом сильно завысил подать, записав в императорские кодексы налог в десять тысяч сто пятьдесят два солида. Так над городом нависли черные тучи. Вскоре они породили страшную бурю, опустошившую родную епархию святителя Николая. Ибо непомерная подать разоряет народ, словно ураган или пожар.
+Когда указ о размере налогов был утвержден в Константинополе, другой царский сановник отправился в Миры с военным отрядом собирать подать. Прибыв в город, он понял: взыскать установленную сумму для казны императора будет крайне сложно. Весь вечер и всю ночь чиновник размышлял, как ему действовать, и решил проявить твердость и даже жестокость при исполнении императорского указа. Утром сборщик налогов воссел на трибунале и начал взимать подать. Требуя деньги, он сильно унижал народ, унижал вплоть до страшных оскорблений. Изо дня в день он так угнетал горожан поборами, так притеснял всех, что обрек ликийцев на разорение и голод.
+Кто мог защитить Миры от крайней нищеты и убедить монарха снизить непомерную подать? Слава о святом угоднике Божьем Николае уже распространилась по всей империи; со времени I Вселенского Собора император Константин знал святителя и почитал его. Поэтому всю свою надежду ликийцы возложили на архиепископа Николая. Подобно тому, как терпящий бедствие корабль устремляется к тихой спасительной гавани, жители города Миры поспешили к мудрому архиерею Божьему. Они припали к его ногам и со слезами просили написать письмо благочестивейшему Государю о беде, случившейся с ними, умолить самодержца сжалиться и уменьшить налоговое бремя. Чадолюбивый отец Николай незамедлительно откликнулся на просьбу о помощи своей униженной и бедствующей паствы.
+– Дети мои возлюбленные, – произнес добрый пастырь, – я не только напишу монарху, но и сам поеду в Константинополь к нашему христолюбивому императору и буду упрашивать его снизить подать, которой чиновник обложил Миры из ненависти и вражды к его жителям.
+Владыка помолился и после недолгих приготовлений отправился в путь. Славный заступник Николай прибыл в Константинополь поздно вечером и остановился при церкви Пресвятой Богородицы[31]. Там, вкусив немного пищи с братией, святитель всю ночь в храме молил Господа смягчить сердце Василевса.
+На рассвете епископы(*), находившиеся в Константинополе, уже знали о прибытии в столицу знаменитого иерарха Николая. Они пришли со свечами и кадильницами в храм Всечестной Владычицы нашей Богородицы и воздали угоднику Божьему подобающую честь. Архиереи припали к ногам святого, прося у него благословения. Преподобный Николай обнял каждого из них и пожелал всем мира. Затем владыки сели. Святитель стал беседовать с епископами и поведал им о жестоком притеснении народа в Ликии царскими сановниками.
+Настал час служения Божественной Литургии. Архиереи попросили всеславного Николая возглавить службу. Во время Таинства, когда богоносный отец произнес: «Святая святым», все в алтаре увидели, как из его уст вышло огненное пламя. С великим страхом они прославили Бога, творящего чудеса через Своих угодников. Народ, собравшийся в храме, причастился Божественных Тайн из ангельских рук светоча Христова. По окончании Литургии миряне разошлись по домам, а владыки и клирики остались со всеми любимым Николаем и с радостью провели с ним весь день. Вечером они снова совершили богослужение, затем долго беседовали со святым и, преклонив головы, дремали до рассвета.
+Утром великий заступник помолился и отправился в царский дворец. Императору доложили о прибытии Мирликийского архиепископа. Государь повелел пропустить к нему владыку. Преподобный служитель Христов вошел в тронный зал и увидел самодержца, восседавшего на троне. Солнце сквозь окно бросало лучи на лицо монарха и слепило ему глаза. Чудотворец Николай снял со своих плеч мантию и накинул ее на солнечный луч, затенив лицо императора. И, о, чудо! Мантия не упала. Все увидели, как она висит в воздухе на солнечном луче, ничем не поддерживаемая. Константин был поражен.
+Он встал с трона, с трепетом поклонился святому, облобызал его и спросил:
+– Раб Бога Вышнего, что привело тебя к нам?
+– Владыка вселенной, – кротко произнес мёдоречивый Николай, – милостью Божьей ныне весь род христианский управляется твоей справедливой десницей. В дни твоего царствования христиане избавлены от насилия и непрестанно возносят за тебя молитвы. Мы, ликийцы, смиренно взирая на Христа, Истинного Бога, также просим Его помочь тебе побеждать иноверных врагов и во всем сопутствовать твоей державе. Когда мы, о, благочестивейший император, благодарили за тебя Господа, радовались и ликовали, коварный враг рода человеческого помешал нам жить в мире и славить Всесильного Бога, даровавшего тебе царство.
+– Что же случилось в Ликии? – спросил Константин.
+– Владыка самодержец! Во время переписи столичный чиновник из-за ненависти и неразумного соперничества то ли со мной, то ли с кем-то из жителей города решил причинить зло моей пастве. По наущению дьявола он обложил податью в десять тысяч сто пятьдесят два солида нашу бедную епархию и убедил твое величество утвердить этот непомерный налог. А другой чиновник, посланный в Миры собирать подать, подверг горожан сильным притеснениям и наказаниям, требуя ее уплаты. Многие ликийцы разорены, впали в крайнюю нищету и страдают от голода. Поэтому беда заставила меня обратиться к твоей благочестивой власти. Прошу, о, император, восстанови справедливость в нашей митрополии.
+Государь с волнением слушал епископа из Ликии. Все это время мантия архиерея висела на солнечном луче. Константин снял мантию, своими царскими руками надел ее на плечи угодника Божьего и посадил высокочтимого гостя около себя напротив трона(*).
+– Святой владыка, – обратился к чудотворцу Николаю христолюбивый император. Нищета и голод в Мирах заставили тебя прийти к нам с ходатайством о снижении налога. Твоя просьба о бедствующем народе услышана нами. Ради твоей святости, дабы Господь сохранил благополучие всей державы, я прикажу убавить налог до суммы, которую ты назовешь.
+– На сколько Бог подвигнет твое царское великодушие, на столько и сократи налог, – кротко ответил Николай.
+Самодержец приказал протонотарию и хартулярию Феодосию принести лист и написать:
+– Жители Мир должны ежегодно выплачивать налог в сто солидов. От остальной подати наше величество освобождает город по просьбе за бедных преподобного Николая.
+Константин подписал документ киноварью, скрепил его золотой печатью и вручил хрисовул святителю. Благочестивый монарх попросил прощения у архиепископа Николая. Государю было стыдно, ибо он по неведению допустил несправедливое притеснение Ликии. А архиерей Божий стал молиться за императора и благодарить его за оказанную милость.
+Покинув царский дворец, славный иерарх вернулся в храм Пресвятой Богородицы и снова с горячей молитвой обратился ко Господу. Прозорливый владыка предвидел, что сановники Василевса будут недовольны значительным снижением налога с ликийцев и постараются уговорить Константина не делать этого. Если же документ окажется в Ликии и будет там обнародован, то самодержец не станет менять сво</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Николай_Чудотворец</t>
+  </si>
+  <si>
+    <t>https://ru.wikipedia.org/wiki/Николай_Чудотворец#/media/Файл:St_Nicholas_Icon_Sinai_13th_century.jpg</t>
+  </si>
+  <si>
+    <t>г. Бари, Италия</t>
   </si>
 </sst>
 </file>
@@ -5068,7 +5759,7 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5096,6 +5787,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -5128,7 +5831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -5146,6 +5849,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
@@ -5449,13 +6164,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V83"/>
+  <dimension ref="A1:V138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B62" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5480,7 +6195,7 @@
     <col min="18" max="18" width="12.5703125" customWidth="1"/>
     <col min="19" max="19" width="17.42578125" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" customWidth="1"/>
-    <col min="21" max="21" width="20.7109375" customWidth="1"/>
+    <col min="21" max="21" width="32.42578125" customWidth="1"/>
     <col min="22" max="22" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5603,7 +6318,7 @@
       <c r="R2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="17" t="s">
         <v>32</v>
       </c>
       <c r="T2" s="2" t="s">
@@ -10080,11 +10795,909 @@
         <v>953</v>
       </c>
     </row>
-    <row r="81" ht="15" customHeight="1"/>
-    <row r="82" ht="15" customHeight="1"/>
-    <row r="83" ht="15" customHeight="1"/>
+    <row r="81" spans="1:22" ht="15" customHeight="1">
+      <c r="A81" s="13"/>
+      <c r="B81" s="13" t="s">
+        <v>1042</v>
+      </c>
+      <c r="C81" s="13"/>
+      <c r="D81" s="13" t="s">
+        <v>1043</v>
+      </c>
+      <c r="E81" s="13" t="s">
+        <v>1044</v>
+      </c>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>1045</v>
+      </c>
+      <c r="I81" s="13" t="s">
+        <v>1046</v>
+      </c>
+      <c r="J81" s="13" t="s">
+        <v>1047</v>
+      </c>
+      <c r="K81" s="13"/>
+      <c r="L81" s="13"/>
+      <c r="M81" s="13"/>
+      <c r="N81" s="13" t="s">
+        <v>1048</v>
+      </c>
+      <c r="O81" s="13" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P81" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q81" s="14" t="s">
+        <v>1050</v>
+      </c>
+      <c r="R81" s="15" t="s">
+        <v>1051</v>
+      </c>
+      <c r="S81" s="15" t="s">
+        <v>1052</v>
+      </c>
+      <c r="T81" s="13" t="s">
+        <v>1053</v>
+      </c>
+      <c r="U81" s="13"/>
+      <c r="V81" s="13"/>
+    </row>
+    <row r="82" spans="1:22" ht="15" customHeight="1">
+      <c r="A82" s="13"/>
+      <c r="B82" s="13" t="s">
+        <v>1054</v>
+      </c>
+      <c r="C82" s="13"/>
+      <c r="D82" s="13" t="s">
+        <v>1055</v>
+      </c>
+      <c r="E82" s="13" t="s">
+        <v>1056</v>
+      </c>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="H82" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="I82" s="13" t="s">
+        <v>1058</v>
+      </c>
+      <c r="J82" s="13" t="s">
+        <v>1057</v>
+      </c>
+      <c r="K82" s="13" t="s">
+        <v>1044</v>
+      </c>
+      <c r="L82" s="13" t="s">
+        <v>1059</v>
+      </c>
+      <c r="M82" s="13"/>
+      <c r="N82" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="O82" s="13" t="s">
+        <v>1060</v>
+      </c>
+      <c r="P82" s="13" t="s">
+        <v>1061</v>
+      </c>
+      <c r="Q82" s="14" t="s">
+        <v>1062</v>
+      </c>
+      <c r="R82" s="15" t="s">
+        <v>1063</v>
+      </c>
+      <c r="S82" s="15" t="s">
+        <v>1064</v>
+      </c>
+      <c r="T82" s="13" t="s">
+        <v>1065</v>
+      </c>
+      <c r="U82" s="13"/>
+      <c r="V82" s="13"/>
+    </row>
+    <row r="83" spans="1:22" ht="15" customHeight="1">
+      <c r="A83" s="13"/>
+      <c r="B83" s="13" t="s">
+        <v>1066</v>
+      </c>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13" t="s">
+        <v>1067</v>
+      </c>
+      <c r="E83" s="13" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="13"/>
+      <c r="L83" s="13"/>
+      <c r="M83" s="13"/>
+      <c r="N83" s="13" t="s">
+        <v>1070</v>
+      </c>
+      <c r="O83" s="16" t="s">
+        <v>1071</v>
+      </c>
+      <c r="P83" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q83" s="14" t="s">
+        <v>1072</v>
+      </c>
+      <c r="R83" s="15" t="s">
+        <v>1073</v>
+      </c>
+      <c r="S83" s="15" t="s">
+        <v>1074</v>
+      </c>
+      <c r="T83" s="13" t="s">
+        <v>1075</v>
+      </c>
+      <c r="U83" s="13"/>
+      <c r="V83" s="13"/>
+    </row>
+    <row r="84" spans="1:22" ht="15" customHeight="1">
+      <c r="A84" s="13"/>
+      <c r="B84" s="13" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E84" s="13" t="s">
+        <v>1078</v>
+      </c>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I84" s="13" t="s">
+        <v>1079</v>
+      </c>
+      <c r="J84" s="13" t="s">
+        <v>1080</v>
+      </c>
+      <c r="K84" s="13"/>
+      <c r="L84" s="13"/>
+      <c r="M84" s="13"/>
+      <c r="N84" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O84" s="13" t="s">
+        <v>1081</v>
+      </c>
+      <c r="P84" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q84" s="14" t="s">
+        <v>1082</v>
+      </c>
+      <c r="R84" s="15" t="s">
+        <v>1083</v>
+      </c>
+      <c r="S84" s="15" t="s">
+        <v>1084</v>
+      </c>
+      <c r="T84" s="13" t="s">
+        <v>1085</v>
+      </c>
+      <c r="U84" s="13"/>
+      <c r="V84" s="13"/>
+    </row>
+    <row r="85" spans="1:22" ht="15" customHeight="1">
+      <c r="A85" s="13"/>
+      <c r="B85" s="13" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13" t="s">
+        <v>1087</v>
+      </c>
+      <c r="E85" s="13" t="s">
+        <v>1088</v>
+      </c>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>1089</v>
+      </c>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+      <c r="L85" s="13"/>
+      <c r="M85" s="13"/>
+      <c r="N85" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="O85" s="13" t="s">
+        <v>1090</v>
+      </c>
+      <c r="P85" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q85" s="14" t="s">
+        <v>1091</v>
+      </c>
+      <c r="R85" s="15" t="s">
+        <v>1092</v>
+      </c>
+      <c r="S85" s="15" t="s">
+        <v>1093</v>
+      </c>
+      <c r="T85" s="13" t="s">
+        <v>1094</v>
+      </c>
+      <c r="U85" s="13" t="s">
+        <v>1095</v>
+      </c>
+      <c r="V85" s="13"/>
+    </row>
+    <row r="86" spans="1:22" ht="15" customHeight="1">
+      <c r="A86" s="13"/>
+      <c r="B86" s="13" t="s">
+        <v>1096</v>
+      </c>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13" t="s">
+        <v>1097</v>
+      </c>
+      <c r="E86" s="13" t="s">
+        <v>1098</v>
+      </c>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13" t="s">
+        <v>1099</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>1100</v>
+      </c>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="13"/>
+      <c r="L86" s="13"/>
+      <c r="M86" s="13"/>
+      <c r="N86" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O86" s="13" t="s">
+        <v>1101</v>
+      </c>
+      <c r="P86" s="13" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q86" s="14" t="s">
+        <v>1103</v>
+      </c>
+      <c r="R86" s="15" t="s">
+        <v>1104</v>
+      </c>
+      <c r="S86" s="15" t="s">
+        <v>1105</v>
+      </c>
+      <c r="T86" s="13" t="s">
+        <v>1106</v>
+      </c>
+      <c r="U86" s="13"/>
+      <c r="V86" s="13"/>
+    </row>
+    <row r="87" spans="1:22" ht="15" customHeight="1">
+      <c r="A87" s="13"/>
+      <c r="B87" s="13" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C87" s="13"/>
+      <c r="D87" s="13" t="s">
+        <v>1108</v>
+      </c>
+      <c r="E87" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13" t="s">
+        <v>1098</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>1109</v>
+      </c>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
+      <c r="M87" s="13"/>
+      <c r="N87" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O87" s="13" t="s">
+        <v>1110</v>
+      </c>
+      <c r="P87" s="13" t="s">
+        <v>1111</v>
+      </c>
+      <c r="Q87" s="14" t="s">
+        <v>1112</v>
+      </c>
+      <c r="R87" s="15" t="s">
+        <v>1113</v>
+      </c>
+      <c r="S87" s="15" t="s">
+        <v>1114</v>
+      </c>
+      <c r="T87" s="13" t="s">
+        <v>1115</v>
+      </c>
+      <c r="U87" s="13"/>
+      <c r="V87" s="13"/>
+    </row>
+    <row r="88" spans="1:22" ht="15" customHeight="1">
+      <c r="A88" s="13"/>
+      <c r="B88" s="13" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C88" s="13"/>
+      <c r="D88" s="13" t="s">
+        <v>1117</v>
+      </c>
+      <c r="E88" s="13" t="s">
+        <v>1118</v>
+      </c>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O88" s="13" t="s">
+        <v>1120</v>
+      </c>
+      <c r="P88" s="13" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q88" s="14" t="s">
+        <v>1121</v>
+      </c>
+      <c r="R88" s="15" t="s">
+        <v>1122</v>
+      </c>
+      <c r="S88" s="15" t="s">
+        <v>1123</v>
+      </c>
+      <c r="T88" s="13" t="s">
+        <v>1124</v>
+      </c>
+      <c r="U88" s="13"/>
+      <c r="V88" s="13"/>
+    </row>
+    <row r="89" spans="1:22" ht="15" customHeight="1">
+      <c r="A89" s="13"/>
+      <c r="B89" s="13" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C89" s="13"/>
+      <c r="D89" s="13" t="s">
+        <v>1126</v>
+      </c>
+      <c r="E89" s="13" t="s">
+        <v>702</v>
+      </c>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H89" s="13" t="s">
+        <v>1128</v>
+      </c>
+      <c r="I89" s="13" t="s">
+        <v>1129</v>
+      </c>
+      <c r="J89" s="13" t="s">
+        <v>1130</v>
+      </c>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="13" t="s">
+        <v>1131</v>
+      </c>
+      <c r="N89" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O89" s="13" t="s">
+        <v>1132</v>
+      </c>
+      <c r="P89" s="13" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q89" s="14" t="s">
+        <v>1133</v>
+      </c>
+      <c r="R89" s="15" t="s">
+        <v>1134</v>
+      </c>
+      <c r="S89" s="15" t="s">
+        <v>1135</v>
+      </c>
+      <c r="T89" s="13" t="s">
+        <v>1136</v>
+      </c>
+      <c r="U89" s="13"/>
+      <c r="V89" s="13"/>
+    </row>
+    <row r="90" spans="1:22" ht="15" customHeight="1">
+      <c r="A90" s="13"/>
+      <c r="B90" s="13" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C90" s="13"/>
+      <c r="D90" s="13" t="s">
+        <v>1138</v>
+      </c>
+      <c r="E90" s="13" t="s">
+        <v>1139</v>
+      </c>
+      <c r="F90" s="13"/>
+      <c r="G90" s="13" t="s">
+        <v>1140</v>
+      </c>
+      <c r="H90" s="13"/>
+      <c r="I90" s="13"/>
+      <c r="J90" s="13"/>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="13" t="s">
+        <v>1141</v>
+      </c>
+      <c r="N90" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="O90" s="13" t="s">
+        <v>1142</v>
+      </c>
+      <c r="P90" s="13" t="s">
+        <v>1143</v>
+      </c>
+      <c r="Q90" s="14" t="s">
+        <v>1144</v>
+      </c>
+      <c r="R90" s="15" t="s">
+        <v>1145</v>
+      </c>
+      <c r="S90" s="15" t="s">
+        <v>1146</v>
+      </c>
+      <c r="T90" s="13" t="s">
+        <v>1147</v>
+      </c>
+      <c r="U90" s="13"/>
+      <c r="V90" s="13"/>
+    </row>
+    <row r="91" spans="1:22" ht="15" customHeight="1">
+      <c r="A91" s="13"/>
+      <c r="B91" s="13" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C91" s="13"/>
+      <c r="D91" s="13" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E91" s="13" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F91" s="13"/>
+      <c r="G91" s="13" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H91" s="13" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I91" s="13"/>
+      <c r="J91" s="13"/>
+      <c r="K91" s="13"/>
+      <c r="L91" s="13"/>
+      <c r="M91" s="13"/>
+      <c r="N91" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O91" s="13" t="s">
+        <v>1153</v>
+      </c>
+      <c r="P91" s="13" t="s">
+        <v>1102</v>
+      </c>
+      <c r="Q91" s="14" t="s">
+        <v>1154</v>
+      </c>
+      <c r="R91" s="15" t="s">
+        <v>1155</v>
+      </c>
+      <c r="S91" s="15" t="s">
+        <v>1156</v>
+      </c>
+      <c r="T91" s="13" t="s">
+        <v>1157</v>
+      </c>
+      <c r="U91" s="13"/>
+      <c r="V91" s="13"/>
+    </row>
+    <row r="92" spans="1:22" ht="15" customHeight="1">
+      <c r="A92" s="18"/>
+      <c r="B92" s="18" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C92" s="18"/>
+      <c r="D92" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E92" s="18" t="s">
+        <v>1160</v>
+      </c>
+      <c r="F92" s="18"/>
+      <c r="G92" s="18" t="s">
+        <v>1160</v>
+      </c>
+      <c r="H92" s="18" t="s">
+        <v>1161</v>
+      </c>
+      <c r="I92" s="18" t="s">
+        <v>1162</v>
+      </c>
+      <c r="J92" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="K92" s="18" t="s">
+        <v>1163</v>
+      </c>
+      <c r="L92" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="M92" s="18"/>
+      <c r="N92" s="18" t="s">
+        <v>1164</v>
+      </c>
+      <c r="O92" s="18" t="s">
+        <v>1165</v>
+      </c>
+      <c r="P92" s="18" t="s">
+        <v>1166</v>
+      </c>
+      <c r="Q92" s="19" t="s">
+        <v>1167</v>
+      </c>
+      <c r="R92" s="20" t="s">
+        <v>1168</v>
+      </c>
+      <c r="S92" s="20" t="s">
+        <v>1169</v>
+      </c>
+      <c r="T92" s="18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="U92" s="18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="V92" s="18"/>
+    </row>
+    <row r="93" spans="1:22" ht="15" customHeight="1">
+      <c r="A93" s="18"/>
+      <c r="B93" s="18" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C93" s="18"/>
+      <c r="D93" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E93" s="18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="F93" s="18"/>
+      <c r="G93" s="18" t="s">
+        <v>1173</v>
+      </c>
+      <c r="H93" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="I93" s="18"/>
+      <c r="J93" s="18"/>
+      <c r="K93" s="18"/>
+      <c r="L93" s="18"/>
+      <c r="M93" s="18"/>
+      <c r="N93" s="18" t="s">
+        <v>1164</v>
+      </c>
+      <c r="O93" s="18" t="s">
+        <v>1174</v>
+      </c>
+      <c r="P93" s="18" t="s">
+        <v>1166</v>
+      </c>
+      <c r="Q93" s="19" t="s">
+        <v>1175</v>
+      </c>
+      <c r="R93" s="18" t="s">
+        <v>1176</v>
+      </c>
+      <c r="S93" s="20" t="s">
+        <v>1177</v>
+      </c>
+      <c r="T93" s="18" t="s">
+        <v>1159</v>
+      </c>
+      <c r="U93" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="V93" s="18"/>
+    </row>
+    <row r="94" spans="1:22" ht="15" customHeight="1">
+      <c r="A94" s="18"/>
+      <c r="B94" s="18" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C94" s="18"/>
+      <c r="D94" s="18" t="s">
+        <v>1179</v>
+      </c>
+      <c r="E94" s="18" t="s">
+        <v>1180</v>
+      </c>
+      <c r="F94" s="18"/>
+      <c r="G94" s="18" t="s">
+        <v>1180</v>
+      </c>
+      <c r="H94" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I94" s="18"/>
+      <c r="J94" s="18"/>
+      <c r="K94" s="18"/>
+      <c r="L94" s="18"/>
+      <c r="M94" s="18" t="s">
+        <v>1182</v>
+      </c>
+      <c r="N94" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O94" s="18" t="s">
+        <v>1183</v>
+      </c>
+      <c r="P94" s="18" t="s">
+        <v>1184</v>
+      </c>
+      <c r="Q94" s="19" t="s">
+        <v>1185</v>
+      </c>
+      <c r="R94" s="20" t="s">
+        <v>1186</v>
+      </c>
+      <c r="S94" s="20" t="s">
+        <v>1187</v>
+      </c>
+      <c r="T94" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="U94" s="18"/>
+      <c r="V94" s="18"/>
+    </row>
+    <row r="95" spans="1:22" ht="15" customHeight="1">
+      <c r="A95" s="18"/>
+      <c r="B95" s="18" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C95" s="18"/>
+      <c r="D95" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="E95" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F95" s="18"/>
+      <c r="G95" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="H95" s="18" t="s">
+        <v>1181</v>
+      </c>
+      <c r="I95" s="18"/>
+      <c r="J95" s="18"/>
+      <c r="K95" s="18"/>
+      <c r="L95" s="18"/>
+      <c r="M95" s="18"/>
+      <c r="N95" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="O95" s="18" t="s">
+        <v>1191</v>
+      </c>
+      <c r="P95" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q95" s="19" t="s">
+        <v>1192</v>
+      </c>
+      <c r="R95" s="20" t="s">
+        <v>1193</v>
+      </c>
+      <c r="S95" s="20" t="s">
+        <v>1194</v>
+      </c>
+      <c r="T95" s="18" t="s">
+        <v>1195</v>
+      </c>
+      <c r="U95" s="18" t="s">
+        <v>1190</v>
+      </c>
+      <c r="V95" s="18"/>
+    </row>
+    <row r="96" spans="1:22" ht="15" customHeight="1">
+      <c r="A96" s="18"/>
+      <c r="B96" s="18" t="s">
+        <v>1196</v>
+      </c>
+      <c r="C96" s="18"/>
+      <c r="D96" s="18" t="s">
+        <v>1197</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>1198</v>
+      </c>
+      <c r="F96" s="18"/>
+      <c r="G96" s="18" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I96" s="18"/>
+      <c r="J96" s="18"/>
+      <c r="K96" s="18"/>
+      <c r="L96" s="18"/>
+      <c r="M96" s="18"/>
+      <c r="N96" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O96" s="18" t="s">
+        <v>1200</v>
+      </c>
+      <c r="P96" s="18" t="s">
+        <v>1201</v>
+      </c>
+      <c r="Q96" s="19" t="s">
+        <v>1202</v>
+      </c>
+      <c r="R96" s="20" t="s">
+        <v>1203</v>
+      </c>
+      <c r="S96" s="20" t="s">
+        <v>1204</v>
+      </c>
+      <c r="T96" s="18" t="s">
+        <v>1205</v>
+      </c>
+      <c r="U96" s="18" t="s">
+        <v>1206</v>
+      </c>
+      <c r="V96" s="18"/>
+    </row>
+    <row r="97" spans="1:22" ht="15" customHeight="1">
+      <c r="A97" s="18"/>
+      <c r="B97" s="18" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C97" s="18"/>
+      <c r="D97" s="18" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E97" s="18" t="s">
+        <v>1208</v>
+      </c>
+      <c r="F97" s="18"/>
+      <c r="G97" s="18" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H97" s="18" t="s">
+        <v>1182</v>
+      </c>
+      <c r="I97" s="18" t="s">
+        <v>1210</v>
+      </c>
+      <c r="J97" s="18" t="s">
+        <v>1182</v>
+      </c>
+      <c r="K97" s="18"/>
+      <c r="L97" s="18"/>
+      <c r="M97" s="18"/>
+      <c r="N97" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="O97" s="18" t="s">
+        <v>1211</v>
+      </c>
+      <c r="P97" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q97" s="19" t="s">
+        <v>1212</v>
+      </c>
+      <c r="R97" s="20" t="s">
+        <v>1213</v>
+      </c>
+      <c r="S97" s="20" t="s">
+        <v>1214</v>
+      </c>
+      <c r="T97" s="18"/>
+      <c r="U97" s="18" t="s">
+        <v>1215</v>
+      </c>
+      <c r="V97" s="18"/>
+    </row>
+    <row r="98" spans="1:22" ht="15" customHeight="1"/>
+    <row r="99" spans="1:22" ht="15" customHeight="1"/>
+    <row r="100" spans="1:22" ht="15" customHeight="1"/>
+    <row r="101" spans="1:22" ht="15" customHeight="1"/>
+    <row r="102" spans="1:22" ht="15" customHeight="1"/>
+    <row r="103" spans="1:22" ht="15" customHeight="1"/>
+    <row r="104" spans="1:22" ht="15" customHeight="1"/>
+    <row r="105" spans="1:22" ht="15" customHeight="1"/>
+    <row r="106" spans="1:22" ht="15" customHeight="1"/>
+    <row r="107" spans="1:22" ht="15" customHeight="1"/>
+    <row r="108" spans="1:22" ht="15" customHeight="1"/>
+    <row r="109" spans="1:22" ht="15" customHeight="1"/>
+    <row r="110" spans="1:22" ht="15" customHeight="1"/>
+    <row r="111" spans="1:22" ht="15" customHeight="1"/>
+    <row r="112" spans="1:22" ht="15" customHeight="1"/>
+    <row r="113" ht="15" customHeight="1"/>
+    <row r="114" ht="15" customHeight="1"/>
+    <row r="115" ht="15" customHeight="1"/>
+    <row r="116" ht="15" customHeight="1"/>
+    <row r="117" ht="15" customHeight="1"/>
+    <row r="118" ht="15" customHeight="1"/>
+    <row r="119" ht="15" customHeight="1"/>
+    <row r="120" ht="15" customHeight="1"/>
+    <row r="121" ht="15" customHeight="1"/>
+    <row r="122" ht="15" customHeight="1"/>
+    <row r="123" ht="15" customHeight="1"/>
+    <row r="124" ht="15" customHeight="1"/>
+    <row r="125" ht="15" customHeight="1"/>
+    <row r="126" ht="15" customHeight="1"/>
+    <row r="127" ht="15" customHeight="1"/>
+    <row r="128" ht="15" customHeight="1"/>
+    <row r="129" ht="15" customHeight="1"/>
+    <row r="130" ht="15" customHeight="1"/>
+    <row r="131" ht="15" customHeight="1"/>
+    <row r="132" ht="15" customHeight="1"/>
+    <row r="133" ht="15" customHeight="1"/>
+    <row r="134" ht="15" customHeight="1"/>
+    <row r="135" ht="15" customHeight="1"/>
+    <row r="136" ht="15" customHeight="1"/>
+    <row r="137" ht="15" customHeight="1"/>
+    <row r="138" ht="15" customHeight="1"/>
   </sheetData>
-  <autoFilter ref="A1:V1"/>
+  <autoFilter ref="A1:V97"/>
   <hyperlinks>
     <hyperlink ref="R59" r:id="rId1"/>
     <hyperlink ref="R60" r:id="rId2"/>
@@ -10128,9 +11741,43 @@
     <hyperlink ref="R79" r:id="rId39"/>
     <hyperlink ref="S80" r:id="rId40"/>
     <hyperlink ref="R80" r:id="rId41"/>
+    <hyperlink ref="S81" r:id="rId42" location="/media/Файл:Pope_Clement_I.jpg"/>
+    <hyperlink ref="R81" r:id="rId43" location="Житие_Святого_Климента"/>
+    <hyperlink ref="S82" r:id="rId44" location="/media/Файл:Justin_filozof.jpg"/>
+    <hyperlink ref="R82" r:id="rId45"/>
+    <hyperlink ref="S83" r:id="rId46" location="/media/Файл:Heiliger_Cyprianus.jpg"/>
+    <hyperlink ref="R83" r:id="rId47"/>
+    <hyperlink ref="S84" r:id="rId48" location="/media/Файл:Basil_of_Caesarea_icon.jpg"/>
+    <hyperlink ref="R84" r:id="rId49"/>
+    <hyperlink ref="S85" r:id="rId50" location="/media/Файл:Johnchrysostom.jpg"/>
+    <hyperlink ref="R85" r:id="rId51"/>
+    <hyperlink ref="S86" r:id="rId52" location="/media/Файл:Statua_S_Barsanofio_Oria.jpg"/>
+    <hyperlink ref="R86" r:id="rId53"/>
+    <hyperlink ref="S87" r:id="rId54" location="/media/Файл:John_Climacus.jpg"/>
+    <hyperlink ref="R87" r:id="rId55" location="Иконография"/>
+    <hyperlink ref="S88" r:id="rId56" location="/media/Файл:Ioann_Damaskin_ikona.jpg"/>
+    <hyperlink ref="R88" r:id="rId57"/>
+    <hyperlink ref="S89" r:id="rId58" location="/media/Файл:Studite.jpg"/>
+    <hyperlink ref="R89" r:id="rId59"/>
+    <hyperlink ref="S90" r:id="rId60" location="/media/Файл:Votivni_obraz_Ocko_-_Ludmila.jpg"/>
+    <hyperlink ref="R90" r:id="rId61"/>
+    <hyperlink ref="S91" r:id="rId62" location="/media/Файл:Simeon_novyj.jpg"/>
+    <hyperlink ref="R91" r:id="rId63"/>
+    <hyperlink ref="S2" r:id="rId64" location="/media/%D0%A4%D0%B0%D0%B9%D0%BB:Photo_Amvrosiy_Optinskiy.jpg"/>
+    <hyperlink ref="R92" r:id="rId65"/>
+    <hyperlink ref="S92" r:id="rId66" location="/media/Файл:Hosios_Loukas_(diakonikon,_arch)_-_Dionysius_Areopagite.jpg"/>
+    <hyperlink ref="S93" r:id="rId67" location="/media/Файл:Hermes_of_Philippopolis.jpg"/>
+    <hyperlink ref="R94" r:id="rId68"/>
+    <hyperlink ref="S94" r:id="rId69" location="/media/Файл:Grigorii_chudotvoretz.jpg"/>
+    <hyperlink ref="S95" r:id="rId70" location="/media/File:Franciscan-Sisters-Saint-Cecilia-window-vocations-fscc-calledtobe.org.jpg"/>
+    <hyperlink ref="R95" r:id="rId71"/>
+    <hyperlink ref="R96" r:id="rId72"/>
+    <hyperlink ref="S96" r:id="rId73" location="/media/Файл:Sv_Gr_Bogoslov_Simonopetra_kr18v.jpg"/>
+    <hyperlink ref="R97" r:id="rId74"/>
+    <hyperlink ref="S97" r:id="rId75" location="/media/Файл:St_Nicholas_Icon_Sinai_13th_century.jpg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId42"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId76"/>
 </worksheet>
 </file>
 

</xml_diff>